<commit_message>
new data 2025 03 10
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8683" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8727" uniqueCount="578">
   <si>
     <t>Fecha</t>
   </si>
@@ -1762,6 +1762,12 @@
   <si>
     <t>Boros Midrange</t>
   </si>
+  <si>
+    <t>2025.10.03</t>
+  </si>
+  <si>
+    <t>Oct_2025</t>
+  </si>
 </sst>
 </file>
 
@@ -2098,10 +2104,10 @@
   <dimension ref="A1:M2178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2120" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2135" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F2121" sqref="F2121"/>
+      <selection pane="bottomRight" activeCell="F1942" sqref="F1942"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -88228,67 +88234,463 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2145" spans="1:2" ht="15" customHeight="1">
-      <c r="A2145" s="6"/>
-      <c r="B2145" s="7"/>
-    </row>
-    <row r="2146" spans="1:2" ht="15" customHeight="1">
-      <c r="A2146" s="6"/>
-      <c r="B2146" s="7"/>
-    </row>
-    <row r="2147" spans="1:2" ht="15" customHeight="1">
-      <c r="A2147" s="6"/>
-      <c r="B2147" s="7"/>
-    </row>
-    <row r="2148" spans="1:2" ht="15" customHeight="1">
-      <c r="A2148" s="6"/>
-      <c r="B2148" s="7"/>
-    </row>
-    <row r="2149" spans="1:2" ht="15" customHeight="1">
-      <c r="A2149" s="6"/>
-      <c r="B2149" s="7"/>
-    </row>
-    <row r="2150" spans="1:2" ht="15" customHeight="1">
-      <c r="A2150" s="6"/>
-      <c r="B2150" s="7"/>
-    </row>
-    <row r="2151" spans="1:2" ht="15" customHeight="1">
-      <c r="A2151" s="6"/>
-      <c r="B2151" s="7"/>
-    </row>
-    <row r="2152" spans="1:2" ht="15" customHeight="1">
-      <c r="A2152" s="6"/>
-      <c r="B2152" s="7"/>
-    </row>
-    <row r="2153" spans="1:2" ht="15" customHeight="1">
-      <c r="A2153" s="6"/>
-      <c r="B2153" s="7"/>
-    </row>
-    <row r="2154" spans="1:2" ht="15" customHeight="1">
-      <c r="A2154" s="6"/>
-      <c r="B2154" s="7"/>
-    </row>
-    <row r="2155" spans="1:2" ht="15" customHeight="1">
-      <c r="A2155" s="6"/>
-      <c r="B2155" s="7"/>
-    </row>
-    <row r="2156" spans="1:2" ht="15" customHeight="1">
+    <row r="2145" spans="1:13" ht="15" customHeight="1">
+      <c r="A2145" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2145" s="7">
+        <v>160</v>
+      </c>
+      <c r="C2145">
+        <v>1</v>
+      </c>
+      <c r="D2145" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2145">
+        <v>14</v>
+      </c>
+      <c r="F2145" t="s">
+        <v>378</v>
+      </c>
+      <c r="H2145" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2145">
+        <v>2</v>
+      </c>
+      <c r="J2145">
+        <v>0</v>
+      </c>
+      <c r="K2145">
+        <v>1</v>
+      </c>
+      <c r="L2145" t="str">
+        <f t="shared" ref="L2145:L2155" si="83">IF(C2145=1,"1",IF(C2145=2,"1",IF(C2145=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2145" t="str">
+        <f t="shared" ref="M2145:M2155" si="84">IF(C2145=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2146" spans="1:13" ht="15" customHeight="1">
+      <c r="A2146" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2146" s="7">
+        <v>160</v>
+      </c>
+      <c r="C2146">
+        <v>2</v>
+      </c>
+      <c r="D2146" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2146">
+        <v>14</v>
+      </c>
+      <c r="F2146" t="s">
+        <v>163</v>
+      </c>
+      <c r="H2146" t="s">
+        <v>452</v>
+      </c>
+      <c r="I2146">
+        <v>2</v>
+      </c>
+      <c r="J2146">
+        <v>1</v>
+      </c>
+      <c r="K2146">
+        <v>0</v>
+      </c>
+      <c r="L2146" t="str">
+        <f t="shared" si="83"/>
+        <v>1</v>
+      </c>
+      <c r="M2146" t="str">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2147" spans="1:13" ht="15" customHeight="1">
+      <c r="A2147" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2147" s="7">
+        <v>160</v>
+      </c>
+      <c r="C2147">
+        <v>3</v>
+      </c>
+      <c r="D2147" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2147">
+        <v>14</v>
+      </c>
+      <c r="F2147" t="s">
+        <v>553</v>
+      </c>
+      <c r="H2147" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2147">
+        <v>2</v>
+      </c>
+      <c r="J2147">
+        <v>1</v>
+      </c>
+      <c r="K2147">
+        <v>0</v>
+      </c>
+      <c r="L2147" t="str">
+        <f t="shared" si="83"/>
+        <v>1</v>
+      </c>
+      <c r="M2147" t="str">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2148" spans="1:13" ht="15" customHeight="1">
+      <c r="A2148" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2148" s="7">
+        <v>160</v>
+      </c>
+      <c r="C2148">
+        <v>4</v>
+      </c>
+      <c r="D2148" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2148">
+        <v>14</v>
+      </c>
+      <c r="F2148" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2148" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2148">
+        <v>2</v>
+      </c>
+      <c r="J2148">
+        <v>1</v>
+      </c>
+      <c r="K2148">
+        <v>0</v>
+      </c>
+      <c r="L2148" t="str">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="M2148" t="str">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2149" spans="1:13" ht="15" customHeight="1">
+      <c r="A2149" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2149" s="7">
+        <v>160</v>
+      </c>
+      <c r="C2149">
+        <v>5</v>
+      </c>
+      <c r="D2149" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2149">
+        <v>14</v>
+      </c>
+      <c r="F2149" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2149" t="s">
+        <v>313</v>
+      </c>
+      <c r="I2149">
+        <v>2</v>
+      </c>
+      <c r="J2149">
+        <v>1</v>
+      </c>
+      <c r="K2149">
+        <v>0</v>
+      </c>
+      <c r="L2149" t="str">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="M2149" t="str">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2150" spans="1:13" ht="15" customHeight="1">
+      <c r="A2150" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2150" s="7">
+        <v>160</v>
+      </c>
+      <c r="C2150">
+        <v>6</v>
+      </c>
+      <c r="D2150" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2150">
+        <v>14</v>
+      </c>
+      <c r="F2150" t="s">
+        <v>394</v>
+      </c>
+      <c r="H2150" t="s">
+        <v>215</v>
+      </c>
+      <c r="I2150">
+        <v>1</v>
+      </c>
+      <c r="J2150">
+        <v>1</v>
+      </c>
+      <c r="K2150">
+        <v>1</v>
+      </c>
+      <c r="L2150" t="str">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="M2150" t="str">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2151" spans="1:13" ht="15" customHeight="1">
+      <c r="A2151" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2151" s="7">
+        <v>160</v>
+      </c>
+      <c r="C2151">
+        <v>7</v>
+      </c>
+      <c r="D2151" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2151">
+        <v>14</v>
+      </c>
+      <c r="F2151" t="s">
+        <v>573</v>
+      </c>
+      <c r="H2151" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2151">
+        <v>1</v>
+      </c>
+      <c r="J2151">
+        <v>2</v>
+      </c>
+      <c r="K2151">
+        <v>0</v>
+      </c>
+      <c r="L2151" t="str">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="M2151" t="str">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2152" spans="1:13" ht="15" customHeight="1">
+      <c r="A2152" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2152" s="7">
+        <v>160</v>
+      </c>
+      <c r="C2152">
+        <v>8</v>
+      </c>
+      <c r="D2152" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2152">
+        <v>14</v>
+      </c>
+      <c r="F2152" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2152" t="s">
+        <v>570</v>
+      </c>
+      <c r="I2152">
+        <v>1</v>
+      </c>
+      <c r="J2152">
+        <v>2</v>
+      </c>
+      <c r="K2152">
+        <v>0</v>
+      </c>
+      <c r="L2152" t="str">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="M2152" t="str">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2153" spans="1:13" ht="15" customHeight="1">
+      <c r="A2153" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2153" s="7">
+        <v>160</v>
+      </c>
+      <c r="C2153">
+        <v>9</v>
+      </c>
+      <c r="D2153" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2153">
+        <v>14</v>
+      </c>
+      <c r="F2153" t="s">
+        <v>225</v>
+      </c>
+      <c r="H2153" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2153">
+        <v>1</v>
+      </c>
+      <c r="J2153">
+        <v>2</v>
+      </c>
+      <c r="K2153">
+        <v>0</v>
+      </c>
+      <c r="L2153" t="str">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="M2153" t="str">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2154" spans="1:13" ht="15" customHeight="1">
+      <c r="A2154" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2154" s="7">
+        <v>160</v>
+      </c>
+      <c r="C2154">
+        <v>10</v>
+      </c>
+      <c r="D2154" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2154">
+        <v>14</v>
+      </c>
+      <c r="F2154" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2154" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2154">
+        <v>1</v>
+      </c>
+      <c r="J2154">
+        <v>2</v>
+      </c>
+      <c r="K2154">
+        <v>0</v>
+      </c>
+      <c r="L2154" t="str">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="M2154" t="str">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2155" spans="1:13" ht="15" customHeight="1">
+      <c r="A2155" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2155" s="7">
+        <v>160</v>
+      </c>
+      <c r="C2155">
+        <v>11</v>
+      </c>
+      <c r="D2155" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2155">
+        <v>14</v>
+      </c>
+      <c r="F2155" t="s">
+        <v>512</v>
+      </c>
+      <c r="H2155" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2155">
+        <v>1</v>
+      </c>
+      <c r="J2155">
+        <v>2</v>
+      </c>
+      <c r="K2155">
+        <v>0</v>
+      </c>
+      <c r="L2155" t="str">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="M2155" t="str">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2156" spans="1:13" ht="15" customHeight="1">
       <c r="A2156" s="6"/>
       <c r="B2156" s="7"/>
     </row>
-    <row r="2157" spans="1:2" ht="15" customHeight="1">
+    <row r="2157" spans="1:13" ht="15" customHeight="1">
       <c r="A2157" s="6"/>
       <c r="B2157" s="7"/>
     </row>
-    <row r="2158" spans="1:2" ht="15" customHeight="1">
+    <row r="2158" spans="1:13" ht="15" customHeight="1">
       <c r="A2158" s="6"/>
       <c r="B2158" s="7"/>
     </row>
-    <row r="2159" spans="1:2" ht="15" customHeight="1">
+    <row r="2159" spans="1:13" ht="15" customHeight="1">
       <c r="A2159" s="6"/>
       <c r="B2159" s="7"/>
     </row>
-    <row r="2160" spans="1:2" ht="15" customHeight="1">
+    <row r="2160" spans="1:13" ht="15" customHeight="1">
       <c r="A2160" s="6"/>
       <c r="B2160" s="7"/>
     </row>

</xml_diff>

<commit_message>
new data 2025 10 10
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8727" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8861" uniqueCount="589">
   <si>
     <t>Fecha</t>
   </si>
@@ -1768,6 +1768,39 @@
   <si>
     <t>Oct_2025</t>
   </si>
+  <si>
+    <t>2025.10.06</t>
+  </si>
+  <si>
+    <t>2025.10.10</t>
+  </si>
+  <si>
+    <t>Gabriel Berrios</t>
+  </si>
+  <si>
+    <t>Francisco Ibañez</t>
+  </si>
+  <si>
+    <t>Marcelo Lamilla</t>
+  </si>
+  <si>
+    <t>Paulo Gonzalez</t>
+  </si>
+  <si>
+    <t>Jorge Pardo</t>
+  </si>
+  <si>
+    <t>Gaspar Allende</t>
+  </si>
+  <si>
+    <t>Mono G Tokens</t>
+  </si>
+  <si>
+    <t>Lucas Vogel</t>
+  </si>
+  <si>
+    <t>Dimir Affinity</t>
+  </si>
 </sst>
 </file>
 
@@ -2101,13 +2134,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2178"/>
+  <dimension ref="A1:M2188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2135" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F1942" sqref="F1942"/>
+      <selection pane="bottomRight" activeCell="F2189" sqref="F2189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -88675,96 +88708,1330 @@
       </c>
     </row>
     <row r="2156" spans="1:13" ht="15" customHeight="1">
-      <c r="A2156" s="6"/>
-      <c r="B2156" s="7"/>
+      <c r="A2156" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2156" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2156">
+        <v>1</v>
+      </c>
+      <c r="D2156" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2156">
+        <v>14</v>
+      </c>
+      <c r="F2156" t="s">
+        <v>446</v>
+      </c>
+      <c r="H2156" t="s">
+        <v>308</v>
+      </c>
+      <c r="I2156">
+        <v>3</v>
+      </c>
+      <c r="J2156">
+        <v>0</v>
+      </c>
+      <c r="K2156">
+        <v>0</v>
+      </c>
+      <c r="L2156" t="str">
+        <f t="shared" ref="L2156:L2188" si="85">IF(C2156=1,"1",IF(C2156=2,"1",IF(C2156=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2156" t="str">
+        <f t="shared" ref="M2156:M2188" si="86">IF(C2156=1,"1","0")</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="2157" spans="1:13" ht="15" customHeight="1">
-      <c r="A2157" s="6"/>
-      <c r="B2157" s="7"/>
+      <c r="A2157" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2157" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2157">
+        <v>2</v>
+      </c>
+      <c r="D2157" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2157">
+        <v>14</v>
+      </c>
+      <c r="F2157" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2157" t="s">
+        <v>313</v>
+      </c>
+      <c r="I2157">
+        <v>2</v>
+      </c>
+      <c r="J2157">
+        <v>0</v>
+      </c>
+      <c r="K2157">
+        <v>1</v>
+      </c>
+      <c r="L2157" t="str">
+        <f t="shared" si="85"/>
+        <v>1</v>
+      </c>
+      <c r="M2157" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="2158" spans="1:13" ht="15" customHeight="1">
-      <c r="A2158" s="6"/>
-      <c r="B2158" s="7"/>
+      <c r="A2158" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2158" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2158">
+        <v>3</v>
+      </c>
+      <c r="D2158" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2158">
+        <v>14</v>
+      </c>
+      <c r="F2158" t="s">
+        <v>512</v>
+      </c>
+      <c r="H2158" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2158">
+        <v>2</v>
+      </c>
+      <c r="J2158">
+        <v>1</v>
+      </c>
+      <c r="K2158">
+        <v>0</v>
+      </c>
+      <c r="L2158" t="str">
+        <f t="shared" si="85"/>
+        <v>1</v>
+      </c>
+      <c r="M2158" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="2159" spans="1:13" ht="15" customHeight="1">
-      <c r="A2159" s="6"/>
-      <c r="B2159" s="7"/>
+      <c r="A2159" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2159" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2159">
+        <v>4</v>
+      </c>
+      <c r="D2159" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2159">
+        <v>14</v>
+      </c>
+      <c r="F2159" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2159" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2159">
+        <v>2</v>
+      </c>
+      <c r="J2159">
+        <v>1</v>
+      </c>
+      <c r="K2159">
+        <v>0</v>
+      </c>
+      <c r="L2159" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2159" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="2160" spans="1:13" ht="15" customHeight="1">
-      <c r="A2160" s="6"/>
-      <c r="B2160" s="7"/>
-    </row>
-    <row r="2161" spans="1:2" ht="15" customHeight="1">
-      <c r="A2161" s="6"/>
-      <c r="B2161" s="7"/>
-    </row>
-    <row r="2162" spans="1:2" ht="15" customHeight="1">
-      <c r="A2162" s="6"/>
-      <c r="B2162" s="7"/>
-    </row>
-    <row r="2163" spans="1:2" ht="15" customHeight="1">
-      <c r="A2163" s="6"/>
-      <c r="B2163" s="7"/>
-    </row>
-    <row r="2164" spans="1:2" ht="15" customHeight="1">
-      <c r="A2164" s="6"/>
-      <c r="B2164" s="7"/>
-    </row>
-    <row r="2165" spans="1:2" ht="15" customHeight="1">
-      <c r="A2165" s="6"/>
-      <c r="B2165" s="7"/>
-    </row>
-    <row r="2166" spans="1:2" ht="15" customHeight="1">
-      <c r="A2166" s="6"/>
-      <c r="B2166" s="7"/>
-    </row>
-    <row r="2167" spans="1:2" ht="15" customHeight="1">
-      <c r="A2167" s="6"/>
-      <c r="B2167" s="7"/>
-    </row>
-    <row r="2168" spans="1:2" ht="15" customHeight="1">
-      <c r="A2168" s="6"/>
-      <c r="B2168" s="7"/>
-    </row>
-    <row r="2169" spans="1:2" ht="15" customHeight="1">
-      <c r="A2169" s="6"/>
-      <c r="B2169" s="7"/>
-    </row>
-    <row r="2170" spans="1:2" ht="15" customHeight="1">
-      <c r="A2170" s="6"/>
-      <c r="B2170" s="7"/>
-    </row>
-    <row r="2171" spans="1:2" ht="15" customHeight="1">
-      <c r="A2171" s="6"/>
-      <c r="B2171" s="7"/>
-    </row>
-    <row r="2172" spans="1:2" ht="15" customHeight="1">
-      <c r="A2172" s="6"/>
-      <c r="B2172" s="7"/>
-    </row>
-    <row r="2173" spans="1:2" ht="15" customHeight="1">
-      <c r="A2173" s="6"/>
-      <c r="B2173" s="7"/>
-    </row>
-    <row r="2174" spans="1:2" ht="15" customHeight="1">
-      <c r="A2174" s="6"/>
-      <c r="B2174" s="7"/>
-    </row>
-    <row r="2175" spans="1:2" ht="15" customHeight="1">
-      <c r="A2175" s="6"/>
-      <c r="B2175" s="7"/>
-    </row>
-    <row r="2176" spans="1:2" ht="15" customHeight="1">
-      <c r="A2176" s="6"/>
-      <c r="B2176" s="7"/>
-    </row>
-    <row r="2177" spans="1:2" ht="15" customHeight="1">
-      <c r="A2177" s="6"/>
-      <c r="B2177" s="7"/>
-    </row>
-    <row r="2178" spans="1:2" ht="15" customHeight="1">
-      <c r="A2178" s="6"/>
-      <c r="B2178" s="7"/>
+      <c r="A2160" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2160" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2160">
+        <v>5</v>
+      </c>
+      <c r="D2160" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2160">
+        <v>14</v>
+      </c>
+      <c r="F2160" t="s">
+        <v>378</v>
+      </c>
+      <c r="H2160" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2160">
+        <v>2</v>
+      </c>
+      <c r="J2160">
+        <v>1</v>
+      </c>
+      <c r="K2160">
+        <v>0</v>
+      </c>
+      <c r="L2160" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2160" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2161" spans="1:13" ht="15" customHeight="1">
+      <c r="A2161" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2161" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2161">
+        <v>6</v>
+      </c>
+      <c r="D2161" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2161">
+        <v>14</v>
+      </c>
+      <c r="F2161" t="s">
+        <v>553</v>
+      </c>
+      <c r="H2161" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2161">
+        <v>2</v>
+      </c>
+      <c r="J2161">
+        <v>1</v>
+      </c>
+      <c r="K2161">
+        <v>0</v>
+      </c>
+      <c r="L2161" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2161" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2162" spans="1:13" ht="15" customHeight="1">
+      <c r="A2162" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2162" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2162">
+        <v>7</v>
+      </c>
+      <c r="D2162" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2162">
+        <v>14</v>
+      </c>
+      <c r="F2162" t="s">
+        <v>512</v>
+      </c>
+      <c r="H2162" t="s">
+        <v>141</v>
+      </c>
+      <c r="I2162">
+        <v>2</v>
+      </c>
+      <c r="J2162">
+        <v>1</v>
+      </c>
+      <c r="K2162">
+        <v>0</v>
+      </c>
+      <c r="L2162" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2162" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2163" spans="1:13" ht="15" customHeight="1">
+      <c r="A2163" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2163" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2163">
+        <v>8</v>
+      </c>
+      <c r="D2163" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2163">
+        <v>14</v>
+      </c>
+      <c r="F2163" t="s">
+        <v>397</v>
+      </c>
+      <c r="H2163" t="s">
+        <v>580</v>
+      </c>
+      <c r="I2163">
+        <v>1</v>
+      </c>
+      <c r="J2163">
+        <v>1</v>
+      </c>
+      <c r="K2163">
+        <v>1</v>
+      </c>
+      <c r="L2163" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2163" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2164" spans="1:13" ht="15" customHeight="1">
+      <c r="A2164" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2164" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2164">
+        <v>9</v>
+      </c>
+      <c r="D2164" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2164">
+        <v>14</v>
+      </c>
+      <c r="F2164" t="s">
+        <v>573</v>
+      </c>
+      <c r="H2164" t="s">
+        <v>581</v>
+      </c>
+      <c r="I2164">
+        <v>1</v>
+      </c>
+      <c r="J2164">
+        <v>1</v>
+      </c>
+      <c r="K2164">
+        <v>1</v>
+      </c>
+      <c r="L2164" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2164" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2165" spans="1:13" ht="15" customHeight="1">
+      <c r="A2165" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2165" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2165">
+        <v>10</v>
+      </c>
+      <c r="D2165" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2165">
+        <v>14</v>
+      </c>
+      <c r="F2165" t="s">
+        <v>586</v>
+      </c>
+      <c r="H2165" t="s">
+        <v>582</v>
+      </c>
+      <c r="I2165">
+        <v>1</v>
+      </c>
+      <c r="J2165">
+        <v>2</v>
+      </c>
+      <c r="K2165">
+        <v>0</v>
+      </c>
+      <c r="L2165" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2165" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2166" spans="1:13" ht="15" customHeight="1">
+      <c r="A2166" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2166" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2166">
+        <v>11</v>
+      </c>
+      <c r="D2166" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2166">
+        <v>14</v>
+      </c>
+      <c r="F2166" t="s">
+        <v>397</v>
+      </c>
+      <c r="H2166" t="s">
+        <v>583</v>
+      </c>
+      <c r="I2166">
+        <v>1</v>
+      </c>
+      <c r="J2166">
+        <v>2</v>
+      </c>
+      <c r="K2166">
+        <v>0</v>
+      </c>
+      <c r="L2166" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2166" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2167" spans="1:13" ht="15" customHeight="1">
+      <c r="A2167" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2167" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2167">
+        <v>12</v>
+      </c>
+      <c r="D2167" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2167">
+        <v>14</v>
+      </c>
+      <c r="F2167" t="s">
+        <v>394</v>
+      </c>
+      <c r="H2167" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2167">
+        <v>1</v>
+      </c>
+      <c r="J2167">
+        <v>2</v>
+      </c>
+      <c r="K2167">
+        <v>0</v>
+      </c>
+      <c r="L2167" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2167" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2168" spans="1:13" ht="15" customHeight="1">
+      <c r="A2168" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2168" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2168">
+        <v>13</v>
+      </c>
+      <c r="D2168" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2168">
+        <v>14</v>
+      </c>
+      <c r="F2168" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2168" t="s">
+        <v>584</v>
+      </c>
+      <c r="I2168">
+        <v>1</v>
+      </c>
+      <c r="J2168">
+        <v>2</v>
+      </c>
+      <c r="K2168">
+        <v>0</v>
+      </c>
+      <c r="L2168" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2168" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2169" spans="1:13" ht="15" customHeight="1">
+      <c r="A2169" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2169" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2169">
+        <v>14</v>
+      </c>
+      <c r="D2169" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2169">
+        <v>14</v>
+      </c>
+      <c r="F2169" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2169" t="s">
+        <v>546</v>
+      </c>
+      <c r="H2169" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2169">
+        <v>0</v>
+      </c>
+      <c r="J2169">
+        <v>2</v>
+      </c>
+      <c r="K2169">
+        <v>1</v>
+      </c>
+      <c r="L2169" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2169" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2170" spans="1:13" ht="15" customHeight="1">
+      <c r="A2170" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2170" s="7">
+        <v>161</v>
+      </c>
+      <c r="C2170">
+        <v>15</v>
+      </c>
+      <c r="D2170" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2170">
+        <v>14</v>
+      </c>
+      <c r="F2170" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2170" t="s">
+        <v>585</v>
+      </c>
+      <c r="I2170">
+        <v>0</v>
+      </c>
+      <c r="J2170">
+        <v>3</v>
+      </c>
+      <c r="K2170">
+        <v>0</v>
+      </c>
+      <c r="L2170" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2170" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2171" spans="1:13" ht="15" customHeight="1">
+      <c r="A2171" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2171" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2171">
+        <v>1</v>
+      </c>
+      <c r="D2171" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2171">
+        <v>14</v>
+      </c>
+      <c r="F2171" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2171" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2171">
+        <v>3</v>
+      </c>
+      <c r="J2171">
+        <v>0</v>
+      </c>
+      <c r="K2171">
+        <v>0</v>
+      </c>
+      <c r="L2171" t="str">
+        <f t="shared" si="85"/>
+        <v>1</v>
+      </c>
+      <c r="M2171" t="str">
+        <f t="shared" si="86"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2172" spans="1:13" ht="15" customHeight="1">
+      <c r="A2172" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2172" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2172">
+        <v>2</v>
+      </c>
+      <c r="D2172" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2172">
+        <v>14</v>
+      </c>
+      <c r="F2172" t="s">
+        <v>378</v>
+      </c>
+      <c r="H2172" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2172">
+        <v>3</v>
+      </c>
+      <c r="J2172">
+        <v>0</v>
+      </c>
+      <c r="K2172">
+        <v>0</v>
+      </c>
+      <c r="L2172" t="str">
+        <f t="shared" si="85"/>
+        <v>1</v>
+      </c>
+      <c r="M2172" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2173" spans="1:13" ht="15" customHeight="1">
+      <c r="A2173" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2173" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2173">
+        <v>3</v>
+      </c>
+      <c r="D2173" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2173">
+        <v>14</v>
+      </c>
+      <c r="F2173" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2173" t="s">
+        <v>564</v>
+      </c>
+      <c r="I2173">
+        <v>2</v>
+      </c>
+      <c r="J2173">
+        <v>0</v>
+      </c>
+      <c r="K2173">
+        <v>1</v>
+      </c>
+      <c r="L2173" t="str">
+        <f t="shared" si="85"/>
+        <v>1</v>
+      </c>
+      <c r="M2173" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2174" spans="1:13" ht="15" customHeight="1">
+      <c r="A2174" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2174" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2174">
+        <v>4</v>
+      </c>
+      <c r="D2174" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2174">
+        <v>14</v>
+      </c>
+      <c r="F2174" t="s">
+        <v>553</v>
+      </c>
+      <c r="G2174" t="s">
+        <v>562</v>
+      </c>
+      <c r="H2174" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2174">
+        <v>2</v>
+      </c>
+      <c r="J2174">
+        <v>1</v>
+      </c>
+      <c r="K2174">
+        <v>0</v>
+      </c>
+      <c r="L2174" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2174" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2175" spans="1:13" ht="15" customHeight="1">
+      <c r="A2175" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2175" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2175">
+        <v>5</v>
+      </c>
+      <c r="D2175" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2175">
+        <v>14</v>
+      </c>
+      <c r="F2175" t="s">
+        <v>526</v>
+      </c>
+      <c r="H2175" t="s">
+        <v>587</v>
+      </c>
+      <c r="I2175">
+        <v>2</v>
+      </c>
+      <c r="J2175">
+        <v>1</v>
+      </c>
+      <c r="K2175">
+        <v>0</v>
+      </c>
+      <c r="L2175" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2175" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2176" spans="1:13" ht="15" customHeight="1">
+      <c r="A2176" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2176" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2176">
+        <v>6</v>
+      </c>
+      <c r="D2176" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2176">
+        <v>14</v>
+      </c>
+      <c r="F2176" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2176" t="s">
+        <v>570</v>
+      </c>
+      <c r="I2176">
+        <v>2</v>
+      </c>
+      <c r="J2176">
+        <v>1</v>
+      </c>
+      <c r="K2176">
+        <v>0</v>
+      </c>
+      <c r="L2176" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2176" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2177" spans="1:13" ht="15" customHeight="1">
+      <c r="A2177" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2177" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2177">
+        <v>7</v>
+      </c>
+      <c r="D2177" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2177">
+        <v>14</v>
+      </c>
+      <c r="F2177" t="s">
+        <v>163</v>
+      </c>
+      <c r="H2177" t="s">
+        <v>452</v>
+      </c>
+      <c r="I2177">
+        <v>2</v>
+      </c>
+      <c r="J2177">
+        <v>1</v>
+      </c>
+      <c r="K2177">
+        <v>0</v>
+      </c>
+      <c r="L2177" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2177" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2178" spans="1:13" ht="15" customHeight="1">
+      <c r="A2178" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2178" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2178">
+        <v>8</v>
+      </c>
+      <c r="D2178" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2178">
+        <v>14</v>
+      </c>
+      <c r="F2178" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2178" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2178">
+        <v>2</v>
+      </c>
+      <c r="J2178">
+        <v>1</v>
+      </c>
+      <c r="K2178">
+        <v>0</v>
+      </c>
+      <c r="L2178" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2178" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2179" spans="1:13">
+      <c r="A2179" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2179" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2179">
+        <v>9</v>
+      </c>
+      <c r="D2179" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2179">
+        <v>14</v>
+      </c>
+      <c r="F2179" t="s">
+        <v>588</v>
+      </c>
+      <c r="H2179" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2179">
+        <v>2</v>
+      </c>
+      <c r="J2179">
+        <v>1</v>
+      </c>
+      <c r="K2179">
+        <v>0</v>
+      </c>
+      <c r="L2179" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2179" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2180" spans="1:13">
+      <c r="A2180" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2180" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2180">
+        <v>10</v>
+      </c>
+      <c r="D2180" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2180">
+        <v>14</v>
+      </c>
+      <c r="F2180" t="s">
+        <v>553</v>
+      </c>
+      <c r="H2180" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2180">
+        <v>1</v>
+      </c>
+      <c r="J2180">
+        <v>2</v>
+      </c>
+      <c r="K2180">
+        <v>0</v>
+      </c>
+      <c r="L2180" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2180" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2181" spans="1:13">
+      <c r="A2181" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2181" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2181">
+        <v>11</v>
+      </c>
+      <c r="D2181" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2181">
+        <v>14</v>
+      </c>
+      <c r="F2181" t="s">
+        <v>526</v>
+      </c>
+      <c r="H2181" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2181">
+        <v>1</v>
+      </c>
+      <c r="J2181">
+        <v>2</v>
+      </c>
+      <c r="K2181">
+        <v>0</v>
+      </c>
+      <c r="L2181" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2181" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2182" spans="1:13">
+      <c r="A2182" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2182" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2182">
+        <v>12</v>
+      </c>
+      <c r="D2182" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2182">
+        <v>14</v>
+      </c>
+      <c r="F2182" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2182" t="s">
+        <v>262</v>
+      </c>
+      <c r="I2182">
+        <v>1</v>
+      </c>
+      <c r="J2182">
+        <v>2</v>
+      </c>
+      <c r="K2182">
+        <v>0</v>
+      </c>
+      <c r="L2182" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2182" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2183" spans="1:13">
+      <c r="A2183" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2183" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2183">
+        <v>13</v>
+      </c>
+      <c r="D2183" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2183">
+        <v>14</v>
+      </c>
+      <c r="F2183" t="s">
+        <v>394</v>
+      </c>
+      <c r="H2183" t="s">
+        <v>302</v>
+      </c>
+      <c r="I2183">
+        <v>1</v>
+      </c>
+      <c r="J2183">
+        <v>2</v>
+      </c>
+      <c r="K2183">
+        <v>0</v>
+      </c>
+      <c r="L2183" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2183" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2184" spans="1:13">
+      <c r="A2184" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2184" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2184">
+        <v>14</v>
+      </c>
+      <c r="D2184" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2184">
+        <v>14</v>
+      </c>
+      <c r="F2184" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2184" t="s">
+        <v>281</v>
+      </c>
+      <c r="I2184">
+        <v>1</v>
+      </c>
+      <c r="J2184">
+        <v>2</v>
+      </c>
+      <c r="K2184">
+        <v>0</v>
+      </c>
+      <c r="L2184" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2184" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2185" spans="1:13">
+      <c r="A2185" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2185" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2185">
+        <v>15</v>
+      </c>
+      <c r="D2185" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2185">
+        <v>14</v>
+      </c>
+      <c r="F2185" t="s">
+        <v>550</v>
+      </c>
+      <c r="H2185" t="s">
+        <v>313</v>
+      </c>
+      <c r="I2185">
+        <v>0</v>
+      </c>
+      <c r="J2185">
+        <v>2</v>
+      </c>
+      <c r="K2185">
+        <v>1</v>
+      </c>
+      <c r="L2185" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2185" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2186" spans="1:13">
+      <c r="A2186" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2186" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2186">
+        <v>16</v>
+      </c>
+      <c r="D2186" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2186">
+        <v>14</v>
+      </c>
+      <c r="F2186" t="s">
+        <v>588</v>
+      </c>
+      <c r="H2186" t="s">
+        <v>417</v>
+      </c>
+      <c r="I2186">
+        <v>0</v>
+      </c>
+      <c r="J2186">
+        <v>2</v>
+      </c>
+      <c r="K2186">
+        <v>0</v>
+      </c>
+      <c r="L2186" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2186" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2187" spans="1:13">
+      <c r="A2187" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2187" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2187">
+        <v>17</v>
+      </c>
+      <c r="D2187" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2187">
+        <v>14</v>
+      </c>
+      <c r="F2187" t="s">
+        <v>163</v>
+      </c>
+      <c r="H2187" t="s">
+        <v>507</v>
+      </c>
+      <c r="I2187">
+        <v>0</v>
+      </c>
+      <c r="J2187">
+        <v>2</v>
+      </c>
+      <c r="K2187">
+        <v>0</v>
+      </c>
+      <c r="L2187" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2187" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2188" spans="1:13">
+      <c r="A2188" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2188" s="7">
+        <v>162</v>
+      </c>
+      <c r="C2188">
+        <v>18</v>
+      </c>
+      <c r="D2188" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2188">
+        <v>14</v>
+      </c>
+      <c r="F2188" t="s">
+        <v>512</v>
+      </c>
+      <c r="H2188" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2188">
+        <v>0</v>
+      </c>
+      <c r="J2188">
+        <v>3</v>
+      </c>
+      <c r="K2188">
+        <v>0</v>
+      </c>
+      <c r="L2188" t="str">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="M2188" t="str">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Z667"/>

</xml_diff>

<commit_message>
new data octubre antes fly
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8861" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8927" uniqueCount="593">
   <si>
     <t>Fecha</t>
   </si>
@@ -1801,6 +1801,18 @@
   <si>
     <t>Dimir Affinity</t>
   </si>
+  <si>
+    <t>2025.10.17</t>
+  </si>
+  <si>
+    <t>Fabian Aguilar</t>
+  </si>
+  <si>
+    <t>Pablo Cruz</t>
+  </si>
+  <si>
+    <t>con descarte</t>
+  </si>
 </sst>
 </file>
 
@@ -2134,13 +2146,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2188"/>
+  <dimension ref="A1:M2204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2167" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2182" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F2189" sqref="F2189"/>
+      <selection pane="bottomRight" activeCell="F2190" sqref="F2190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -90030,6 +90042,652 @@
       </c>
       <c r="M2188" t="str">
         <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2189" spans="1:13">
+      <c r="A2189" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2189" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2189">
+        <v>1</v>
+      </c>
+      <c r="D2189" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2189">
+        <v>14</v>
+      </c>
+      <c r="F2189" t="s">
+        <v>573</v>
+      </c>
+      <c r="H2189" t="s">
+        <v>305</v>
+      </c>
+      <c r="I2189">
+        <v>3</v>
+      </c>
+      <c r="J2189">
+        <v>0</v>
+      </c>
+      <c r="K2189">
+        <v>0</v>
+      </c>
+      <c r="L2189" t="str">
+        <f t="shared" ref="L2189:L2204" si="87">IF(C2189=1,"1",IF(C2189=2,"1",IF(C2189=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2189" t="str">
+        <f t="shared" ref="M2189:M2204" si="88">IF(C2189=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2190" spans="1:13">
+      <c r="A2190" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2190" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2190">
+        <v>2</v>
+      </c>
+      <c r="D2190" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2190">
+        <v>14</v>
+      </c>
+      <c r="F2190" t="s">
+        <v>526</v>
+      </c>
+      <c r="H2190" t="s">
+        <v>313</v>
+      </c>
+      <c r="I2190">
+        <v>3</v>
+      </c>
+      <c r="J2190">
+        <v>0</v>
+      </c>
+      <c r="K2190">
+        <v>0</v>
+      </c>
+      <c r="L2190" t="str">
+        <f t="shared" si="87"/>
+        <v>1</v>
+      </c>
+      <c r="M2190" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2191" spans="1:13">
+      <c r="A2191" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2191" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2191">
+        <v>3</v>
+      </c>
+      <c r="D2191" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2191">
+        <v>14</v>
+      </c>
+      <c r="F2191" t="s">
+        <v>550</v>
+      </c>
+      <c r="H2191" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2191">
+        <v>2</v>
+      </c>
+      <c r="J2191">
+        <v>0</v>
+      </c>
+      <c r="K2191">
+        <v>1</v>
+      </c>
+      <c r="L2191" t="str">
+        <f t="shared" si="87"/>
+        <v>1</v>
+      </c>
+      <c r="M2191" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2192" spans="1:13">
+      <c r="A2192" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2192" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2192">
+        <v>4</v>
+      </c>
+      <c r="D2192" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2192">
+        <v>14</v>
+      </c>
+      <c r="F2192" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2192" t="s">
+        <v>587</v>
+      </c>
+      <c r="I2192">
+        <v>2</v>
+      </c>
+      <c r="J2192">
+        <v>1</v>
+      </c>
+      <c r="K2192">
+        <v>0</v>
+      </c>
+      <c r="L2192" t="str">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="M2192" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2193" spans="1:13">
+      <c r="A2193" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2193" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2193">
+        <v>5</v>
+      </c>
+      <c r="D2193" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2193">
+        <v>14</v>
+      </c>
+      <c r="F2193" t="s">
+        <v>378</v>
+      </c>
+      <c r="H2193" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2193">
+        <v>2</v>
+      </c>
+      <c r="J2193">
+        <v>1</v>
+      </c>
+      <c r="K2193">
+        <v>0</v>
+      </c>
+      <c r="L2193" t="str">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="M2193" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2194" spans="1:13">
+      <c r="A2194" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2194" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2194">
+        <v>6</v>
+      </c>
+      <c r="D2194" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2194">
+        <v>14</v>
+      </c>
+      <c r="F2194" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2194" t="s">
+        <v>262</v>
+      </c>
+      <c r="I2194">
+        <v>2</v>
+      </c>
+      <c r="J2194">
+        <v>1</v>
+      </c>
+      <c r="K2194">
+        <v>0</v>
+      </c>
+      <c r="L2194" t="str">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="M2194" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2195" spans="1:13">
+      <c r="A2195" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2195" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2195">
+        <v>7</v>
+      </c>
+      <c r="D2195" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2195">
+        <v>14</v>
+      </c>
+      <c r="F2195" t="s">
+        <v>378</v>
+      </c>
+      <c r="G2195" t="s">
+        <v>592</v>
+      </c>
+      <c r="H2195" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2195">
+        <v>2</v>
+      </c>
+      <c r="J2195">
+        <v>1</v>
+      </c>
+      <c r="K2195">
+        <v>0</v>
+      </c>
+      <c r="L2195" t="str">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="M2195" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2196" spans="1:13">
+      <c r="A2196" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2196" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2196">
+        <v>8</v>
+      </c>
+      <c r="D2196" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2196">
+        <v>14</v>
+      </c>
+      <c r="F2196" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2196" t="s">
+        <v>507</v>
+      </c>
+      <c r="I2196">
+        <v>1</v>
+      </c>
+      <c r="J2196">
+        <v>1</v>
+      </c>
+      <c r="K2196">
+        <v>1</v>
+      </c>
+      <c r="L2196" t="str">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="M2196" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2197" spans="1:13">
+      <c r="A2197" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2197" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2197">
+        <v>9</v>
+      </c>
+      <c r="D2197" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2197">
+        <v>14</v>
+      </c>
+      <c r="F2197" t="s">
+        <v>394</v>
+      </c>
+      <c r="H2197" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2197">
+        <v>1</v>
+      </c>
+      <c r="J2197">
+        <v>1</v>
+      </c>
+      <c r="K2197">
+        <v>1</v>
+      </c>
+      <c r="L2197" t="str">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="M2197" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2198" spans="1:13">
+      <c r="A2198" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2198" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2198">
+        <v>10</v>
+      </c>
+      <c r="D2198" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2198">
+        <v>14</v>
+      </c>
+      <c r="F2198" t="s">
+        <v>526</v>
+      </c>
+      <c r="H2198" t="s">
+        <v>417</v>
+      </c>
+      <c r="I2198">
+        <v>1</v>
+      </c>
+      <c r="J2198">
+        <v>2</v>
+      </c>
+      <c r="K2198">
+        <v>0</v>
+      </c>
+      <c r="L2198" t="str">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="M2198" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2199" spans="1:13">
+      <c r="A2199" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2199" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2199">
+        <v>11</v>
+      </c>
+      <c r="D2199" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2199">
+        <v>14</v>
+      </c>
+      <c r="F2199" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2199" t="s">
+        <v>517</v>
+      </c>
+      <c r="H2199" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2199">
+        <v>1</v>
+      </c>
+      <c r="J2199">
+        <v>2</v>
+      </c>
+      <c r="K2199">
+        <v>0</v>
+      </c>
+      <c r="L2199" t="str">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="M2199" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2200" spans="1:13">
+      <c r="A2200" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2200" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2200">
+        <v>12</v>
+      </c>
+      <c r="D2200" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2200">
+        <v>14</v>
+      </c>
+      <c r="F2200" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2200" t="s">
+        <v>590</v>
+      </c>
+      <c r="I2200">
+        <v>1</v>
+      </c>
+      <c r="J2200">
+        <v>2</v>
+      </c>
+      <c r="K2200">
+        <v>0</v>
+      </c>
+      <c r="L2200" t="str">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="M2200" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2201" spans="1:13">
+      <c r="A2201" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2201" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2201">
+        <v>13</v>
+      </c>
+      <c r="D2201" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2201">
+        <v>14</v>
+      </c>
+      <c r="F2201" t="s">
+        <v>553</v>
+      </c>
+      <c r="H2201" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2201">
+        <v>1</v>
+      </c>
+      <c r="J2201">
+        <v>2</v>
+      </c>
+      <c r="K2201">
+        <v>0</v>
+      </c>
+      <c r="L2201" t="str">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="M2201" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2202" spans="1:13">
+      <c r="A2202" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2202" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2202">
+        <v>14</v>
+      </c>
+      <c r="D2202" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2202">
+        <v>14</v>
+      </c>
+      <c r="F2202" t="s">
+        <v>573</v>
+      </c>
+      <c r="H2202" t="s">
+        <v>544</v>
+      </c>
+      <c r="I2202">
+        <v>0</v>
+      </c>
+      <c r="J2202">
+        <v>2</v>
+      </c>
+      <c r="K2202">
+        <v>1</v>
+      </c>
+      <c r="L2202" t="str">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="M2202" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2203" spans="1:13">
+      <c r="A2203" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2203" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2203">
+        <v>15</v>
+      </c>
+      <c r="D2203" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2203">
+        <v>14</v>
+      </c>
+      <c r="F2203" t="s">
+        <v>574</v>
+      </c>
+      <c r="H2203" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2203">
+        <v>0</v>
+      </c>
+      <c r="J2203">
+        <v>1</v>
+      </c>
+      <c r="K2203">
+        <v>0</v>
+      </c>
+      <c r="L2203" t="str">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="M2203" t="str">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2204" spans="1:13">
+      <c r="A2204" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2204" s="7">
+        <v>163</v>
+      </c>
+      <c r="C2204">
+        <v>16</v>
+      </c>
+      <c r="D2204" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2204">
+        <v>14</v>
+      </c>
+      <c r="F2204" t="s">
+        <v>526</v>
+      </c>
+      <c r="H2204" t="s">
+        <v>591</v>
+      </c>
+      <c r="I2204">
+        <v>0</v>
+      </c>
+      <c r="J2204">
+        <v>3</v>
+      </c>
+      <c r="K2204">
+        <v>0</v>
+      </c>
+      <c r="L2204" t="str">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="M2204" t="str">
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new data 2025 11 07
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8927" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8992" uniqueCount="596">
   <si>
     <t>Fecha</t>
   </si>
@@ -1813,6 +1813,15 @@
   <si>
     <t>con descarte</t>
   </si>
+  <si>
+    <t>2025.11.07</t>
+  </si>
+  <si>
+    <t>Nov_2025</t>
+  </si>
+  <si>
+    <t>Fernando Yaksic</t>
+  </si>
 </sst>
 </file>
 
@@ -2146,13 +2155,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2204"/>
+  <dimension ref="A1:M2220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2182" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2205" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F2190" sqref="F2190"/>
+      <selection pane="bottomRight" activeCell="H2227" sqref="H2227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -90688,6 +90697,649 @@
       </c>
       <c r="M2204" t="str">
         <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2205" spans="1:13">
+      <c r="A2205" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2205" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2205">
+        <v>1</v>
+      </c>
+      <c r="D2205" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2205">
+        <v>14</v>
+      </c>
+      <c r="F2205" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2205" t="s">
+        <v>417</v>
+      </c>
+      <c r="I2205">
+        <v>3</v>
+      </c>
+      <c r="J2205">
+        <v>0</v>
+      </c>
+      <c r="K2205">
+        <v>0</v>
+      </c>
+      <c r="L2205" t="str">
+        <f t="shared" ref="L2205:L2220" si="89">IF(C2205=1,"1",IF(C2205=2,"1",IF(C2205=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2205" t="str">
+        <f t="shared" ref="M2205:M2220" si="90">IF(C2205=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2206" spans="1:13">
+      <c r="A2206" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2206" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2206">
+        <v>2</v>
+      </c>
+      <c r="D2206" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2206">
+        <v>14</v>
+      </c>
+      <c r="F2206" t="s">
+        <v>163</v>
+      </c>
+      <c r="H2206" t="s">
+        <v>452</v>
+      </c>
+      <c r="I2206">
+        <v>3</v>
+      </c>
+      <c r="J2206">
+        <v>0</v>
+      </c>
+      <c r="K2206">
+        <v>0</v>
+      </c>
+      <c r="L2206" t="str">
+        <f t="shared" si="89"/>
+        <v>1</v>
+      </c>
+      <c r="M2206" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2207" spans="1:13">
+      <c r="A2207" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2207" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2207">
+        <v>3</v>
+      </c>
+      <c r="D2207" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2207">
+        <v>14</v>
+      </c>
+      <c r="F2207" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2207" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2207">
+        <v>2</v>
+      </c>
+      <c r="J2207">
+        <v>0</v>
+      </c>
+      <c r="K2207">
+        <v>1</v>
+      </c>
+      <c r="L2207" t="str">
+        <f t="shared" si="89"/>
+        <v>1</v>
+      </c>
+      <c r="M2207" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2208" spans="1:13">
+      <c r="A2208" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2208" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2208">
+        <v>4</v>
+      </c>
+      <c r="D2208" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2208">
+        <v>14</v>
+      </c>
+      <c r="F2208" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2208" t="s">
+        <v>464</v>
+      </c>
+      <c r="I2208">
+        <v>2</v>
+      </c>
+      <c r="J2208">
+        <v>1</v>
+      </c>
+      <c r="K2208">
+        <v>0</v>
+      </c>
+      <c r="L2208" t="str">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M2208" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2209" spans="1:13">
+      <c r="A2209" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2209" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2209">
+        <v>5</v>
+      </c>
+      <c r="D2209" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2209">
+        <v>14</v>
+      </c>
+      <c r="F2209" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2209" t="s">
+        <v>507</v>
+      </c>
+      <c r="I2209">
+        <v>2</v>
+      </c>
+      <c r="J2209">
+        <v>1</v>
+      </c>
+      <c r="K2209">
+        <v>0</v>
+      </c>
+      <c r="L2209" t="str">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M2209" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2210" spans="1:13">
+      <c r="A2210" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2210" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2210">
+        <v>6</v>
+      </c>
+      <c r="D2210" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2210">
+        <v>14</v>
+      </c>
+      <c r="F2210" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2210" t="s">
+        <v>215</v>
+      </c>
+      <c r="I2210">
+        <v>2</v>
+      </c>
+      <c r="J2210">
+        <v>1</v>
+      </c>
+      <c r="K2210">
+        <v>0</v>
+      </c>
+      <c r="L2210" t="str">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M2210" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2211" spans="1:13">
+      <c r="A2211" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2211" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2211">
+        <v>7</v>
+      </c>
+      <c r="D2211" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2211">
+        <v>14</v>
+      </c>
+      <c r="F2211" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2211" t="s">
+        <v>439</v>
+      </c>
+      <c r="I2211">
+        <v>2</v>
+      </c>
+      <c r="J2211">
+        <v>1</v>
+      </c>
+      <c r="K2211">
+        <v>0</v>
+      </c>
+      <c r="L2211" t="str">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M2211" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2212" spans="1:13">
+      <c r="A2212" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2212" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2212">
+        <v>8</v>
+      </c>
+      <c r="D2212" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2212">
+        <v>14</v>
+      </c>
+      <c r="F2212" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2212" t="s">
+        <v>549</v>
+      </c>
+      <c r="H2212" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2212">
+        <v>1</v>
+      </c>
+      <c r="J2212">
+        <v>1</v>
+      </c>
+      <c r="K2212">
+        <v>1</v>
+      </c>
+      <c r="L2212" t="str">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M2212" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2213" spans="1:13">
+      <c r="A2213" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2213" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2213">
+        <v>9</v>
+      </c>
+      <c r="D2213" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2213">
+        <v>14</v>
+      </c>
+      <c r="F2213" t="s">
+        <v>573</v>
+      </c>
+      <c r="H2213" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2213">
+        <v>1</v>
+      </c>
+      <c r="J2213">
+        <v>2</v>
+      </c>
+      <c r="K2213">
+        <v>0</v>
+      </c>
+      <c r="L2213" t="str">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M2213" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2214" spans="1:13">
+      <c r="A2214" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2214" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2214">
+        <v>10</v>
+      </c>
+      <c r="D2214" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2214">
+        <v>14</v>
+      </c>
+      <c r="F2214" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2214" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2214">
+        <v>1</v>
+      </c>
+      <c r="J2214">
+        <v>2</v>
+      </c>
+      <c r="K2214">
+        <v>0</v>
+      </c>
+      <c r="L2214" t="str">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M2214" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2215" spans="1:13">
+      <c r="A2215" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2215" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2215">
+        <v>11</v>
+      </c>
+      <c r="D2215" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2215">
+        <v>14</v>
+      </c>
+      <c r="F2215" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2215" t="s">
+        <v>595</v>
+      </c>
+      <c r="I2215">
+        <v>1</v>
+      </c>
+      <c r="J2215">
+        <v>2</v>
+      </c>
+      <c r="K2215">
+        <v>0</v>
+      </c>
+      <c r="L2215" t="str">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M2215" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2216" spans="1:13">
+      <c r="A2216" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2216" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2216">
+        <v>12</v>
+      </c>
+      <c r="D2216" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2216">
+        <v>14</v>
+      </c>
+      <c r="F2216" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2216" t="s">
+        <v>231</v>
+      </c>
+      <c r="I2216">
+        <v>1</v>
+      </c>
+      <c r="J2216">
+        <v>2</v>
+      </c>
+      <c r="K2216">
+        <v>0</v>
+      </c>
+      <c r="L2216" t="str">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M2216" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2217" spans="1:13">
+      <c r="A2217" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2217" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2217">
+        <v>13</v>
+      </c>
+      <c r="D2217" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2217">
+        <v>14</v>
+      </c>
+      <c r="F2217" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2217" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2217">
+        <v>1</v>
+      </c>
+      <c r="J2217">
+        <v>2</v>
+      </c>
+      <c r="K2217">
+        <v>0</v>
+      </c>
+      <c r="L2217" t="str">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M2217" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2218" spans="1:13">
+      <c r="A2218" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2218" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2218">
+        <v>14</v>
+      </c>
+      <c r="D2218" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2218">
+        <v>14</v>
+      </c>
+      <c r="F2218" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2218" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2218">
+        <v>1</v>
+      </c>
+      <c r="J2218">
+        <v>2</v>
+      </c>
+      <c r="K2218">
+        <v>0</v>
+      </c>
+      <c r="L2218" t="str">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M2218" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2219" spans="1:13">
+      <c r="A2219" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2219" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2219">
+        <v>15</v>
+      </c>
+      <c r="D2219" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2219">
+        <v>14</v>
+      </c>
+      <c r="F2219" t="s">
+        <v>394</v>
+      </c>
+      <c r="H2219" t="s">
+        <v>485</v>
+      </c>
+      <c r="I2219">
+        <v>0</v>
+      </c>
+      <c r="J2219">
+        <v>2</v>
+      </c>
+      <c r="K2219">
+        <v>0</v>
+      </c>
+      <c r="L2219" t="str">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M2219" t="str">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2220" spans="1:13">
+      <c r="A2220" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2220" s="7">
+        <v>164</v>
+      </c>
+      <c r="C2220">
+        <v>16</v>
+      </c>
+      <c r="D2220" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2220">
+        <v>14</v>
+      </c>
+      <c r="F2220" t="s">
+        <v>573</v>
+      </c>
+      <c r="H2220" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2220">
+        <v>0</v>
+      </c>
+      <c r="J2220">
+        <v>3</v>
+      </c>
+      <c r="K2220">
+        <v>0</v>
+      </c>
+      <c r="L2220" t="str">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M2220" t="str">
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new data 2025 11 14 + baneo tide
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8992" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9036" uniqueCount="598">
   <si>
     <t>Fecha</t>
   </si>
@@ -1822,6 +1822,12 @@
   <si>
     <t>Fernando Yaksic</t>
   </si>
+  <si>
+    <t>2025.11.14</t>
+  </si>
+  <si>
+    <t>Sebastian Castro</t>
+  </si>
 </sst>
 </file>
 
@@ -2155,13 +2161,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2220"/>
+  <dimension ref="A1:M2231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2205" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2211" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="H2227" sqref="H2227"/>
+      <selection pane="bottomRight" activeCell="F2229" sqref="F2229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -91340,6 +91346,446 @@
       </c>
       <c r="M2220" t="str">
         <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2221" spans="1:13">
+      <c r="A2221" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2221" s="7">
+        <v>165</v>
+      </c>
+      <c r="C2221">
+        <v>1</v>
+      </c>
+      <c r="D2221" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2221">
+        <v>14</v>
+      </c>
+      <c r="F2221" t="s">
+        <v>550</v>
+      </c>
+      <c r="H2221" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2221">
+        <v>3</v>
+      </c>
+      <c r="J2221">
+        <v>0</v>
+      </c>
+      <c r="K2221">
+        <v>0</v>
+      </c>
+      <c r="L2221" t="str">
+        <f t="shared" ref="L2221:L2231" si="91">IF(C2221=1,"1",IF(C2221=2,"1",IF(C2221=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2221" t="str">
+        <f t="shared" ref="M2221:M2231" si="92">IF(C2221=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2222" spans="1:13">
+      <c r="A2222" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2222" s="7">
+        <v>165</v>
+      </c>
+      <c r="C2222">
+        <v>2</v>
+      </c>
+      <c r="D2222" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2222">
+        <v>14</v>
+      </c>
+      <c r="F2222" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2222" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2222">
+        <v>2</v>
+      </c>
+      <c r="J2222">
+        <v>1</v>
+      </c>
+      <c r="K2222">
+        <v>0</v>
+      </c>
+      <c r="L2222" t="str">
+        <f t="shared" si="91"/>
+        <v>1</v>
+      </c>
+      <c r="M2222" t="str">
+        <f t="shared" si="92"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2223" spans="1:13">
+      <c r="A2223" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2223" s="7">
+        <v>165</v>
+      </c>
+      <c r="C2223">
+        <v>3</v>
+      </c>
+      <c r="D2223" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2223">
+        <v>14</v>
+      </c>
+      <c r="F2223" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2223" t="s">
+        <v>542</v>
+      </c>
+      <c r="I2223">
+        <v>2</v>
+      </c>
+      <c r="J2223">
+        <v>1</v>
+      </c>
+      <c r="K2223">
+        <v>0</v>
+      </c>
+      <c r="L2223" t="str">
+        <f t="shared" si="91"/>
+        <v>1</v>
+      </c>
+      <c r="M2223" t="str">
+        <f t="shared" si="92"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2224" spans="1:13">
+      <c r="A2224" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2224" s="7">
+        <v>165</v>
+      </c>
+      <c r="C2224">
+        <v>4</v>
+      </c>
+      <c r="D2224" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2224">
+        <v>14</v>
+      </c>
+      <c r="F2224" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2224" t="s">
+        <v>417</v>
+      </c>
+      <c r="I2224">
+        <v>2</v>
+      </c>
+      <c r="J2224">
+        <v>1</v>
+      </c>
+      <c r="K2224">
+        <v>0</v>
+      </c>
+      <c r="L2224" t="str">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="M2224" t="str">
+        <f t="shared" si="92"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2225" spans="1:13">
+      <c r="A2225" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2225" s="7">
+        <v>165</v>
+      </c>
+      <c r="C2225">
+        <v>5</v>
+      </c>
+      <c r="D2225" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2225">
+        <v>14</v>
+      </c>
+      <c r="F2225" t="s">
+        <v>526</v>
+      </c>
+      <c r="H2225" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2225">
+        <v>2</v>
+      </c>
+      <c r="J2225">
+        <v>1</v>
+      </c>
+      <c r="K2225">
+        <v>0</v>
+      </c>
+      <c r="L2225" t="str">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="M2225" t="str">
+        <f t="shared" si="92"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2226" spans="1:13">
+      <c r="A2226" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2226" s="7">
+        <v>165</v>
+      </c>
+      <c r="C2226">
+        <v>6</v>
+      </c>
+      <c r="D2226" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2226">
+        <v>14</v>
+      </c>
+      <c r="F2226" t="s">
+        <v>573</v>
+      </c>
+      <c r="H2226" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2226">
+        <v>2</v>
+      </c>
+      <c r="J2226">
+        <v>1</v>
+      </c>
+      <c r="K2226">
+        <v>0</v>
+      </c>
+      <c r="L2226" t="str">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="M2226" t="str">
+        <f t="shared" si="92"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2227" spans="1:13">
+      <c r="A2227" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2227" s="7">
+        <v>165</v>
+      </c>
+      <c r="C2227">
+        <v>7</v>
+      </c>
+      <c r="D2227" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2227">
+        <v>14</v>
+      </c>
+      <c r="F2227" t="s">
+        <v>218</v>
+      </c>
+      <c r="H2227" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2227">
+        <v>1</v>
+      </c>
+      <c r="J2227">
+        <v>2</v>
+      </c>
+      <c r="K2227">
+        <v>0</v>
+      </c>
+      <c r="L2227" t="str">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="M2227" t="str">
+        <f t="shared" si="92"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2228" spans="1:13">
+      <c r="A2228" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2228" s="7">
+        <v>165</v>
+      </c>
+      <c r="C2228">
+        <v>8</v>
+      </c>
+      <c r="D2228" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2228">
+        <v>14</v>
+      </c>
+      <c r="F2228" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2228" t="s">
+        <v>597</v>
+      </c>
+      <c r="I2228">
+        <v>1</v>
+      </c>
+      <c r="J2228">
+        <v>2</v>
+      </c>
+      <c r="K2228">
+        <v>0</v>
+      </c>
+      <c r="L2228" t="str">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="M2228" t="str">
+        <f t="shared" si="92"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2229" spans="1:13">
+      <c r="A2229" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2229" s="7">
+        <v>165</v>
+      </c>
+      <c r="C2229">
+        <v>9</v>
+      </c>
+      <c r="D2229" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2229">
+        <v>14</v>
+      </c>
+      <c r="F2229" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2229" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2229">
+        <v>1</v>
+      </c>
+      <c r="J2229">
+        <v>2</v>
+      </c>
+      <c r="K2229">
+        <v>0</v>
+      </c>
+      <c r="L2229" t="str">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="M2229" t="str">
+        <f t="shared" si="92"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2230" spans="1:13">
+      <c r="A2230" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2230" s="7">
+        <v>165</v>
+      </c>
+      <c r="C2230">
+        <v>10</v>
+      </c>
+      <c r="D2230" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2230">
+        <v>14</v>
+      </c>
+      <c r="F2230" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2230" t="s">
+        <v>507</v>
+      </c>
+      <c r="I2230">
+        <v>1</v>
+      </c>
+      <c r="J2230">
+        <v>2</v>
+      </c>
+      <c r="K2230">
+        <v>0</v>
+      </c>
+      <c r="L2230" t="str">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="M2230" t="str">
+        <f t="shared" si="92"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2231" spans="1:13">
+      <c r="A2231" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2231" s="7">
+        <v>165</v>
+      </c>
+      <c r="C2231">
+        <v>11</v>
+      </c>
+      <c r="D2231" t="s">
+        <v>594</v>
+      </c>
+      <c r="E2231">
+        <v>14</v>
+      </c>
+      <c r="F2231" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2231" t="s">
+        <v>583</v>
+      </c>
+      <c r="I2231">
+        <v>0</v>
+      </c>
+      <c r="J2231">
+        <v>3</v>
+      </c>
+      <c r="K2231">
+        <v>0</v>
+      </c>
+      <c r="L2231" t="str">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="M2231" t="str">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correcion en 2025 12 07
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -1844,10 +1844,10 @@
     <t>Dic_2025</t>
   </si>
   <si>
-    <t>2025.15.07</t>
+    <t>Poison Storm</t>
   </si>
   <si>
-    <t>Poison Storm</t>
+    <t>2025.12.07</t>
   </si>
 </sst>
 </file>
@@ -2185,10 +2185,10 @@
   <dimension ref="A1:M2284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2252" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2261" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F2283" sqref="F2283"/>
+      <selection pane="bottomRight" activeCell="D2288" sqref="D2288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -17073,7 +17073,7 @@
         <v>3</v>
       </c>
       <c r="F370" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H370" t="s">
         <v>36</v>
@@ -17833,7 +17833,7 @@
         <v>3</v>
       </c>
       <c r="F389" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H389" t="s">
         <v>36</v>
@@ -29457,7 +29457,7 @@
         <v>4</v>
       </c>
       <c r="F679" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H679" t="s">
         <v>232</v>
@@ -31417,7 +31417,7 @@
         <v>5</v>
       </c>
       <c r="F728" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H728" t="s">
         <v>232</v>
@@ -46144,7 +46144,7 @@
         <v>7</v>
       </c>
       <c r="F1094" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H1094" t="s">
         <v>36</v>
@@ -56257,7 +56257,7 @@
         <v>8</v>
       </c>
       <c r="F1346" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H1346" t="s">
         <v>36</v>
@@ -68379,7 +68379,7 @@
         <v>10</v>
       </c>
       <c r="F1648" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H1648" t="s">
         <v>36</v>
@@ -93212,7 +93212,7 @@
     </row>
     <row r="2267" spans="1:13">
       <c r="A2267" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2267" s="7">
         <v>169</v>
@@ -93255,7 +93255,7 @@
     </row>
     <row r="2268" spans="1:13">
       <c r="A2268" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2268" s="7">
         <v>169</v>
@@ -93295,7 +93295,7 @@
     </row>
     <row r="2269" spans="1:13">
       <c r="A2269" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2269" s="7">
         <v>169</v>
@@ -93335,7 +93335,7 @@
     </row>
     <row r="2270" spans="1:13">
       <c r="A2270" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2270" s="7">
         <v>169</v>
@@ -93350,7 +93350,7 @@
         <v>14</v>
       </c>
       <c r="F2270" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H2270" t="s">
         <v>433</v>
@@ -93375,7 +93375,7 @@
     </row>
     <row r="2271" spans="1:13">
       <c r="A2271" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2271" s="7">
         <v>169</v>
@@ -93415,7 +93415,7 @@
     </row>
     <row r="2272" spans="1:13">
       <c r="A2272" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2272" s="7">
         <v>169</v>
@@ -93455,7 +93455,7 @@
     </row>
     <row r="2273" spans="1:13">
       <c r="A2273" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2273" s="7">
         <v>169</v>
@@ -93495,7 +93495,7 @@
     </row>
     <row r="2274" spans="1:13">
       <c r="A2274" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2274" s="7">
         <v>169</v>
@@ -93535,7 +93535,7 @@
     </row>
     <row r="2275" spans="1:13">
       <c r="A2275" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2275" s="7">
         <v>169</v>
@@ -93575,7 +93575,7 @@
     </row>
     <row r="2276" spans="1:13">
       <c r="A2276" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2276" s="7">
         <v>169</v>
@@ -93615,7 +93615,7 @@
     </row>
     <row r="2277" spans="1:13">
       <c r="A2277" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2277" s="7">
         <v>169</v>
@@ -93655,7 +93655,7 @@
     </row>
     <row r="2278" spans="1:13">
       <c r="A2278" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2278" s="7">
         <v>169</v>
@@ -93695,7 +93695,7 @@
     </row>
     <row r="2279" spans="1:13">
       <c r="A2279" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2279" s="7">
         <v>169</v>
@@ -93735,7 +93735,7 @@
     </row>
     <row r="2280" spans="1:13">
       <c r="A2280" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2280" s="7">
         <v>169</v>
@@ -93775,7 +93775,7 @@
     </row>
     <row r="2281" spans="1:13">
       <c r="A2281" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2281" s="7">
         <v>169</v>
@@ -93815,7 +93815,7 @@
     </row>
     <row r="2282" spans="1:13">
       <c r="A2282" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2282" s="7">
         <v>169</v>
@@ -93855,7 +93855,7 @@
     </row>
     <row r="2283" spans="1:13">
       <c r="A2283" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2283" s="7">
         <v>169</v>
@@ -93895,7 +93895,7 @@
     </row>
     <row r="2284" spans="1:13">
       <c r="A2284" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B2284" s="7">
         <v>169</v>

</xml_diff>

<commit_message>
new data 2025 12 12
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9249" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9278" uniqueCount="606">
   <si>
     <t>Fecha</t>
   </si>
@@ -1849,6 +1849,9 @@
   <si>
     <t>2025.12.07</t>
   </si>
+  <si>
+    <t>2025.12.12</t>
+  </si>
 </sst>
 </file>
 
@@ -2182,13 +2185,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2284"/>
+  <dimension ref="A1:M2291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2261" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2276" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="D2288" sqref="D2288"/>
+      <selection pane="bottomRight" activeCell="F2292" sqref="F2292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -93930,6 +93933,289 @@
       </c>
       <c r="M2284" t="str">
         <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2285" spans="1:13">
+      <c r="A2285" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="B2285" s="7">
+        <v>170</v>
+      </c>
+      <c r="C2285">
+        <v>1</v>
+      </c>
+      <c r="D2285" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2285">
+        <v>14</v>
+      </c>
+      <c r="F2285" t="s">
+        <v>571</v>
+      </c>
+      <c r="H2285" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2285">
+        <v>3</v>
+      </c>
+      <c r="J2285">
+        <v>0</v>
+      </c>
+      <c r="K2285">
+        <v>0</v>
+      </c>
+      <c r="L2285" t="str">
+        <f t="shared" ref="L2285:L2291" si="97">IF(C2285=1,"1",IF(C2285=2,"1",IF(C2285=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2285" t="str">
+        <f t="shared" ref="M2285:M2291" si="98">IF(C2285=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2286" spans="1:13">
+      <c r="A2286" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="B2286" s="7">
+        <v>170</v>
+      </c>
+      <c r="C2286">
+        <v>2</v>
+      </c>
+      <c r="D2286" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2286">
+        <v>14</v>
+      </c>
+      <c r="F2286" t="s">
+        <v>551</v>
+      </c>
+      <c r="G2286" t="s">
+        <v>560</v>
+      </c>
+      <c r="H2286" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2286">
+        <v>2</v>
+      </c>
+      <c r="J2286">
+        <v>1</v>
+      </c>
+      <c r="K2286">
+        <v>0</v>
+      </c>
+      <c r="L2286" t="str">
+        <f t="shared" si="97"/>
+        <v>1</v>
+      </c>
+      <c r="M2286" t="str">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2287" spans="1:13">
+      <c r="A2287" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="B2287" s="7">
+        <v>170</v>
+      </c>
+      <c r="C2287">
+        <v>3</v>
+      </c>
+      <c r="D2287" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2287">
+        <v>14</v>
+      </c>
+      <c r="F2287" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2287" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2287">
+        <v>2</v>
+      </c>
+      <c r="J2287">
+        <v>1</v>
+      </c>
+      <c r="K2287">
+        <v>0</v>
+      </c>
+      <c r="L2287" t="str">
+        <f t="shared" si="97"/>
+        <v>1</v>
+      </c>
+      <c r="M2287" t="str">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2288" spans="1:13">
+      <c r="A2288" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="B2288" s="7">
+        <v>170</v>
+      </c>
+      <c r="C2288">
+        <v>4</v>
+      </c>
+      <c r="D2288" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2288">
+        <v>14</v>
+      </c>
+      <c r="F2288" t="s">
+        <v>396</v>
+      </c>
+      <c r="H2288" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2288">
+        <v>2</v>
+      </c>
+      <c r="J2288">
+        <v>1</v>
+      </c>
+      <c r="K2288">
+        <v>0</v>
+      </c>
+      <c r="L2288" t="str">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="M2288" t="str">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2289" spans="1:13">
+      <c r="A2289" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="B2289" s="7">
+        <v>170</v>
+      </c>
+      <c r="C2289">
+        <v>5</v>
+      </c>
+      <c r="D2289" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2289">
+        <v>14</v>
+      </c>
+      <c r="F2289" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2289" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2289">
+        <v>1</v>
+      </c>
+      <c r="J2289">
+        <v>2</v>
+      </c>
+      <c r="K2289">
+        <v>0</v>
+      </c>
+      <c r="L2289" t="str">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="M2289" t="str">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2290" spans="1:13">
+      <c r="A2290" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="B2290" s="7">
+        <v>170</v>
+      </c>
+      <c r="C2290">
+        <v>6</v>
+      </c>
+      <c r="D2290" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2290">
+        <v>14</v>
+      </c>
+      <c r="F2290" t="s">
+        <v>551</v>
+      </c>
+      <c r="H2290" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2290">
+        <v>1</v>
+      </c>
+      <c r="J2290">
+        <v>2</v>
+      </c>
+      <c r="K2290">
+        <v>0</v>
+      </c>
+      <c r="L2290" t="str">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="M2290" t="str">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2291" spans="1:13">
+      <c r="A2291" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="B2291" s="7">
+        <v>170</v>
+      </c>
+      <c r="C2291">
+        <v>7</v>
+      </c>
+      <c r="D2291" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2291">
+        <v>14</v>
+      </c>
+      <c r="F2291" t="s">
+        <v>571</v>
+      </c>
+      <c r="H2291" t="s">
+        <v>304</v>
+      </c>
+      <c r="I2291">
+        <v>1</v>
+      </c>
+      <c r="J2291">
+        <v>2</v>
+      </c>
+      <c r="K2291">
+        <v>0</v>
+      </c>
+      <c r="L2291" t="str">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="M2291" t="str">
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new data 2025 12 19 y 2025 12 23
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9278" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9363" uniqueCount="610">
   <si>
     <t>Fecha</t>
   </si>
@@ -1852,6 +1852,18 @@
   <si>
     <t>2025.12.12</t>
   </si>
+  <si>
+    <t>2025.12.19</t>
+  </si>
+  <si>
+    <t>Sultai Control</t>
+  </si>
+  <si>
+    <t>2025.12.23</t>
+  </si>
+  <si>
+    <t>Esper Glintblade</t>
+  </si>
 </sst>
 </file>
 
@@ -2185,13 +2197,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2291"/>
+  <dimension ref="A1:M2312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2276" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2285" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F2292" sqref="F2292"/>
+      <selection pane="bottomRight" activeCell="F2302" sqref="F2302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -94216,6 +94228,849 @@
       </c>
       <c r="M2291" t="str">
         <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2292" spans="1:13">
+      <c r="A2292" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B2292" s="7">
+        <v>171</v>
+      </c>
+      <c r="C2292">
+        <v>1</v>
+      </c>
+      <c r="D2292" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2292">
+        <v>14</v>
+      </c>
+      <c r="F2292" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2292" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2292">
+        <v>3</v>
+      </c>
+      <c r="J2292">
+        <v>0</v>
+      </c>
+      <c r="K2292">
+        <v>0</v>
+      </c>
+      <c r="L2292" t="str">
+        <f t="shared" ref="L2292:L2300" si="99">IF(C2292=1,"1",IF(C2292=2,"1",IF(C2292=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2292" t="str">
+        <f t="shared" ref="M2292:M2300" si="100">IF(C2292=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2293" spans="1:13">
+      <c r="A2293" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B2293" s="7">
+        <v>171</v>
+      </c>
+      <c r="C2293">
+        <v>2</v>
+      </c>
+      <c r="D2293" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2293">
+        <v>14</v>
+      </c>
+      <c r="F2293" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2293" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2293">
+        <v>3</v>
+      </c>
+      <c r="J2293">
+        <v>0</v>
+      </c>
+      <c r="K2293">
+        <v>0</v>
+      </c>
+      <c r="L2293" t="str">
+        <f t="shared" si="99"/>
+        <v>1</v>
+      </c>
+      <c r="M2293" t="str">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2294" spans="1:13">
+      <c r="A2294" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B2294" s="7">
+        <v>171</v>
+      </c>
+      <c r="C2294">
+        <v>3</v>
+      </c>
+      <c r="D2294" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2294">
+        <v>14</v>
+      </c>
+      <c r="F2294" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2294" t="s">
+        <v>532</v>
+      </c>
+      <c r="I2294">
+        <v>2</v>
+      </c>
+      <c r="J2294">
+        <v>1</v>
+      </c>
+      <c r="K2294">
+        <v>0</v>
+      </c>
+      <c r="L2294" t="str">
+        <f t="shared" si="99"/>
+        <v>1</v>
+      </c>
+      <c r="M2294" t="str">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2295" spans="1:13">
+      <c r="A2295" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B2295" s="7">
+        <v>171</v>
+      </c>
+      <c r="C2295">
+        <v>4</v>
+      </c>
+      <c r="D2295" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2295">
+        <v>14</v>
+      </c>
+      <c r="F2295" t="s">
+        <v>571</v>
+      </c>
+      <c r="H2295" t="s">
+        <v>304</v>
+      </c>
+      <c r="I2295">
+        <v>2</v>
+      </c>
+      <c r="J2295">
+        <v>1</v>
+      </c>
+      <c r="K2295">
+        <v>0</v>
+      </c>
+      <c r="L2295" t="str">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="M2295" t="str">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2296" spans="1:13">
+      <c r="A2296" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B2296" s="7">
+        <v>171</v>
+      </c>
+      <c r="C2296">
+        <v>5</v>
+      </c>
+      <c r="D2296" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2296">
+        <v>14</v>
+      </c>
+      <c r="F2296" t="s">
+        <v>603</v>
+      </c>
+      <c r="H2296" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2296">
+        <v>1</v>
+      </c>
+      <c r="J2296">
+        <v>2</v>
+      </c>
+      <c r="K2296">
+        <v>0</v>
+      </c>
+      <c r="L2296" t="str">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="M2296" t="str">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2297" spans="1:13">
+      <c r="A2297" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B2297" s="7">
+        <v>171</v>
+      </c>
+      <c r="C2297">
+        <v>6</v>
+      </c>
+      <c r="D2297" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2297">
+        <v>14</v>
+      </c>
+      <c r="F2297" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2297" t="s">
+        <v>416</v>
+      </c>
+      <c r="I2297">
+        <v>1</v>
+      </c>
+      <c r="J2297">
+        <v>2</v>
+      </c>
+      <c r="K2297">
+        <v>0</v>
+      </c>
+      <c r="L2297" t="str">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="M2297" t="str">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2298" spans="1:13">
+      <c r="A2298" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B2298" s="7">
+        <v>171</v>
+      </c>
+      <c r="C2298">
+        <v>7</v>
+      </c>
+      <c r="D2298" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2298">
+        <v>14</v>
+      </c>
+      <c r="F2298" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2298" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2298">
+        <v>1</v>
+      </c>
+      <c r="J2298">
+        <v>2</v>
+      </c>
+      <c r="K2298">
+        <v>0</v>
+      </c>
+      <c r="L2298" t="str">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="M2298" t="str">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2299" spans="1:13">
+      <c r="A2299" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B2299" s="7">
+        <v>171</v>
+      </c>
+      <c r="C2299">
+        <v>8</v>
+      </c>
+      <c r="D2299" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2299">
+        <v>14</v>
+      </c>
+      <c r="F2299" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2299" t="s">
+        <v>239</v>
+      </c>
+      <c r="I2299">
+        <v>1</v>
+      </c>
+      <c r="J2299">
+        <v>2</v>
+      </c>
+      <c r="K2299">
+        <v>0</v>
+      </c>
+      <c r="L2299" t="str">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="M2299" t="str">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2300" spans="1:13">
+      <c r="A2300" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B2300" s="7">
+        <v>171</v>
+      </c>
+      <c r="C2300">
+        <v>9</v>
+      </c>
+      <c r="D2300" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2300">
+        <v>14</v>
+      </c>
+      <c r="F2300" t="s">
+        <v>607</v>
+      </c>
+      <c r="H2300" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2300">
+        <v>1</v>
+      </c>
+      <c r="J2300">
+        <v>2</v>
+      </c>
+      <c r="K2300">
+        <v>0</v>
+      </c>
+      <c r="L2300" t="str">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="M2300" t="str">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2301" spans="1:13">
+      <c r="A2301" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2301" s="7">
+        <v>172</v>
+      </c>
+      <c r="C2301">
+        <v>1</v>
+      </c>
+      <c r="D2301" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2301">
+        <v>14</v>
+      </c>
+      <c r="F2301" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2301" t="s">
+        <v>214</v>
+      </c>
+      <c r="I2301">
+        <v>3</v>
+      </c>
+      <c r="J2301">
+        <v>0</v>
+      </c>
+      <c r="K2301">
+        <v>0</v>
+      </c>
+      <c r="L2301" t="str">
+        <f t="shared" ref="L2301:L2312" si="101">IF(C2301=1,"1",IF(C2301=2,"1",IF(C2301=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2301" t="str">
+        <f t="shared" ref="M2301:M2312" si="102">IF(C2301=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2302" spans="1:13">
+      <c r="A2302" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2302" s="7">
+        <v>172</v>
+      </c>
+      <c r="C2302">
+        <v>2</v>
+      </c>
+      <c r="D2302" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2302">
+        <v>14</v>
+      </c>
+      <c r="F2302" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2302" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2302">
+        <v>2</v>
+      </c>
+      <c r="J2302">
+        <v>1</v>
+      </c>
+      <c r="K2302">
+        <v>0</v>
+      </c>
+      <c r="L2302" t="str">
+        <f t="shared" si="101"/>
+        <v>1</v>
+      </c>
+      <c r="M2302" t="str">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2303" spans="1:13">
+      <c r="A2303" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2303" s="7">
+        <v>172</v>
+      </c>
+      <c r="C2303">
+        <v>3</v>
+      </c>
+      <c r="D2303" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2303">
+        <v>14</v>
+      </c>
+      <c r="F2303" t="s">
+        <v>609</v>
+      </c>
+      <c r="H2303" t="s">
+        <v>307</v>
+      </c>
+      <c r="I2303">
+        <v>2</v>
+      </c>
+      <c r="J2303">
+        <v>1</v>
+      </c>
+      <c r="K2303">
+        <v>0</v>
+      </c>
+      <c r="L2303" t="str">
+        <f t="shared" si="101"/>
+        <v>1</v>
+      </c>
+      <c r="M2303" t="str">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2304" spans="1:13">
+      <c r="A2304" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2304" s="7">
+        <v>172</v>
+      </c>
+      <c r="C2304">
+        <v>4</v>
+      </c>
+      <c r="D2304" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2304">
+        <v>14</v>
+      </c>
+      <c r="F2304" t="s">
+        <v>236</v>
+      </c>
+      <c r="H2304" t="s">
+        <v>540</v>
+      </c>
+      <c r="I2304">
+        <v>2</v>
+      </c>
+      <c r="J2304">
+        <v>1</v>
+      </c>
+      <c r="K2304">
+        <v>0</v>
+      </c>
+      <c r="L2304" t="str">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="M2304" t="str">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2305" spans="1:13">
+      <c r="A2305" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2305" s="7">
+        <v>172</v>
+      </c>
+      <c r="C2305">
+        <v>5</v>
+      </c>
+      <c r="D2305" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2305">
+        <v>14</v>
+      </c>
+      <c r="F2305" t="s">
+        <v>183</v>
+      </c>
+      <c r="H2305" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2305">
+        <v>2</v>
+      </c>
+      <c r="J2305">
+        <v>1</v>
+      </c>
+      <c r="K2305">
+        <v>0</v>
+      </c>
+      <c r="L2305" t="str">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="M2305" t="str">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2306" spans="1:13">
+      <c r="A2306" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2306" s="7">
+        <v>172</v>
+      </c>
+      <c r="C2306">
+        <v>6</v>
+      </c>
+      <c r="D2306" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2306">
+        <v>14</v>
+      </c>
+      <c r="F2306" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2306" t="s">
+        <v>312</v>
+      </c>
+      <c r="I2306">
+        <v>1</v>
+      </c>
+      <c r="J2306">
+        <v>1</v>
+      </c>
+      <c r="K2306">
+        <v>1</v>
+      </c>
+      <c r="L2306" t="str">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="M2306" t="str">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2307" spans="1:13">
+      <c r="A2307" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2307" s="7">
+        <v>172</v>
+      </c>
+      <c r="C2307">
+        <v>7</v>
+      </c>
+      <c r="D2307" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2307">
+        <v>14</v>
+      </c>
+      <c r="F2307" t="s">
+        <v>551</v>
+      </c>
+      <c r="H2307" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2307">
+        <v>1</v>
+      </c>
+      <c r="J2307">
+        <v>1</v>
+      </c>
+      <c r="K2307">
+        <v>1</v>
+      </c>
+      <c r="L2307" t="str">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="M2307" t="str">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2308" spans="1:13">
+      <c r="A2308" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2308" s="7">
+        <v>172</v>
+      </c>
+      <c r="C2308">
+        <v>8</v>
+      </c>
+      <c r="D2308" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2308">
+        <v>14</v>
+      </c>
+      <c r="F2308" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2308" t="s">
+        <v>568</v>
+      </c>
+      <c r="I2308">
+        <v>1</v>
+      </c>
+      <c r="J2308">
+        <v>2</v>
+      </c>
+      <c r="K2308">
+        <v>0</v>
+      </c>
+      <c r="L2308" t="str">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="M2308" t="str">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2309" spans="1:13">
+      <c r="A2309" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2309" s="7">
+        <v>172</v>
+      </c>
+      <c r="C2309">
+        <v>9</v>
+      </c>
+      <c r="D2309" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2309">
+        <v>14</v>
+      </c>
+      <c r="F2309" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2309" t="s">
+        <v>581</v>
+      </c>
+      <c r="I2309">
+        <v>1</v>
+      </c>
+      <c r="J2309">
+        <v>2</v>
+      </c>
+      <c r="K2309">
+        <v>0</v>
+      </c>
+      <c r="L2309" t="str">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="M2309" t="str">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2310" spans="1:13">
+      <c r="A2310" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2310" s="7">
+        <v>172</v>
+      </c>
+      <c r="C2310">
+        <v>10</v>
+      </c>
+      <c r="D2310" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2310">
+        <v>14</v>
+      </c>
+      <c r="F2310" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2310" t="s">
+        <v>263</v>
+      </c>
+      <c r="I2310">
+        <v>1</v>
+      </c>
+      <c r="J2310">
+        <v>2</v>
+      </c>
+      <c r="K2310">
+        <v>0</v>
+      </c>
+      <c r="L2310" t="str">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="M2310" t="str">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2311" spans="1:13">
+      <c r="A2311" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2311" s="7">
+        <v>172</v>
+      </c>
+      <c r="C2311">
+        <v>11</v>
+      </c>
+      <c r="D2311" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2311">
+        <v>14</v>
+      </c>
+      <c r="F2311" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2311" t="s">
+        <v>515</v>
+      </c>
+      <c r="H2311" t="s">
+        <v>542</v>
+      </c>
+      <c r="I2311">
+        <v>1</v>
+      </c>
+      <c r="J2311">
+        <v>2</v>
+      </c>
+      <c r="K2311">
+        <v>0</v>
+      </c>
+      <c r="L2311" t="str">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="M2311" t="str">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2312" spans="1:13">
+      <c r="A2312" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2312" s="7">
+        <v>172</v>
+      </c>
+      <c r="C2312">
+        <v>12</v>
+      </c>
+      <c r="D2312" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2312">
+        <v>14</v>
+      </c>
+      <c r="F2312" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2312" t="s">
+        <v>532</v>
+      </c>
+      <c r="I2312">
+        <v>0</v>
+      </c>
+      <c r="J2312">
+        <v>3</v>
+      </c>
+      <c r="K2312">
+        <v>0</v>
+      </c>
+      <c r="L2312" t="str">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="M2312" t="str">
+        <f t="shared" si="102"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new data 2025 12 26
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9363" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9405" uniqueCount="614">
   <si>
     <t>Fecha</t>
   </si>
@@ -1864,6 +1864,18 @@
   <si>
     <t>Esper Glintblade</t>
   </si>
+  <si>
+    <t>2025.12.26</t>
+  </si>
+  <si>
+    <t>con hadas</t>
+  </si>
+  <si>
+    <t>Christopher Offermann</t>
+  </si>
+  <si>
+    <t>no de lista</t>
+  </si>
 </sst>
 </file>
 
@@ -2197,13 +2209,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2312"/>
+  <dimension ref="A1:M2322"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2285" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2297" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F2302" sqref="F2302"/>
+      <selection pane="bottomRight" activeCell="G2323" sqref="G2323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -95071,6 +95083,412 @@
       </c>
       <c r="M2312" t="str">
         <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2313" spans="1:13">
+      <c r="A2313" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="B2313" s="7">
+        <v>173</v>
+      </c>
+      <c r="C2313">
+        <v>1</v>
+      </c>
+      <c r="D2313" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2313">
+        <v>14</v>
+      </c>
+      <c r="F2313" t="s">
+        <v>586</v>
+      </c>
+      <c r="G2313" t="s">
+        <v>611</v>
+      </c>
+      <c r="H2313" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2313">
+        <v>3</v>
+      </c>
+      <c r="J2313">
+        <v>0</v>
+      </c>
+      <c r="K2313">
+        <v>0</v>
+      </c>
+      <c r="L2313" t="str">
+        <f t="shared" ref="L2313:L2322" si="103">IF(C2313=1,"1",IF(C2313=2,"1",IF(C2313=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2313" t="str">
+        <f t="shared" ref="M2313:M2322" si="104">IF(C2313=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2314" spans="1:13">
+      <c r="A2314" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="B2314" s="7">
+        <v>173</v>
+      </c>
+      <c r="C2314">
+        <v>2</v>
+      </c>
+      <c r="D2314" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2314">
+        <v>14</v>
+      </c>
+      <c r="F2314" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2314" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2314">
+        <v>3</v>
+      </c>
+      <c r="J2314">
+        <v>0</v>
+      </c>
+      <c r="K2314">
+        <v>0</v>
+      </c>
+      <c r="L2314" t="str">
+        <f t="shared" si="103"/>
+        <v>1</v>
+      </c>
+      <c r="M2314" t="str">
+        <f t="shared" si="104"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2315" spans="1:13">
+      <c r="A2315" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="B2315" s="7">
+        <v>173</v>
+      </c>
+      <c r="C2315">
+        <v>3</v>
+      </c>
+      <c r="D2315" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2315">
+        <v>14</v>
+      </c>
+      <c r="F2315" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2315" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2315">
+        <v>2</v>
+      </c>
+      <c r="J2315">
+        <v>1</v>
+      </c>
+      <c r="K2315">
+        <v>0</v>
+      </c>
+      <c r="L2315" t="str">
+        <f t="shared" si="103"/>
+        <v>1</v>
+      </c>
+      <c r="M2315" t="str">
+        <f t="shared" si="104"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2316" spans="1:13">
+      <c r="A2316" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="B2316" s="7">
+        <v>173</v>
+      </c>
+      <c r="C2316">
+        <v>4</v>
+      </c>
+      <c r="D2316" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2316">
+        <v>14</v>
+      </c>
+      <c r="F2316" t="s">
+        <v>236</v>
+      </c>
+      <c r="H2316" t="s">
+        <v>540</v>
+      </c>
+      <c r="I2316">
+        <v>1</v>
+      </c>
+      <c r="J2316">
+        <v>1</v>
+      </c>
+      <c r="K2316">
+        <v>1</v>
+      </c>
+      <c r="L2316" t="str">
+        <f t="shared" si="103"/>
+        <v>0</v>
+      </c>
+      <c r="M2316" t="str">
+        <f t="shared" si="104"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2317" spans="1:13">
+      <c r="A2317" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="B2317" s="7">
+        <v>173</v>
+      </c>
+      <c r="C2317">
+        <v>5</v>
+      </c>
+      <c r="D2317" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2317">
+        <v>14</v>
+      </c>
+      <c r="F2317" t="s">
+        <v>163</v>
+      </c>
+      <c r="H2317" t="s">
+        <v>532</v>
+      </c>
+      <c r="I2317">
+        <v>1</v>
+      </c>
+      <c r="J2317">
+        <v>1</v>
+      </c>
+      <c r="K2317">
+        <v>1</v>
+      </c>
+      <c r="L2317" t="str">
+        <f t="shared" si="103"/>
+        <v>0</v>
+      </c>
+      <c r="M2317" t="str">
+        <f t="shared" si="104"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2318" spans="1:13">
+      <c r="A2318" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="B2318" s="7">
+        <v>173</v>
+      </c>
+      <c r="C2318">
+        <v>6</v>
+      </c>
+      <c r="D2318" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2318">
+        <v>14</v>
+      </c>
+      <c r="F2318" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2318" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2318">
+        <v>1</v>
+      </c>
+      <c r="J2318">
+        <v>2</v>
+      </c>
+      <c r="K2318">
+        <v>0</v>
+      </c>
+      <c r="L2318" t="str">
+        <f t="shared" si="103"/>
+        <v>0</v>
+      </c>
+      <c r="M2318" t="str">
+        <f t="shared" si="104"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2319" spans="1:13">
+      <c r="A2319" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="B2319" s="7">
+        <v>173</v>
+      </c>
+      <c r="C2319">
+        <v>7</v>
+      </c>
+      <c r="D2319" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2319">
+        <v>14</v>
+      </c>
+      <c r="F2319" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2319" t="s">
+        <v>416</v>
+      </c>
+      <c r="I2319">
+        <v>1</v>
+      </c>
+      <c r="J2319">
+        <v>2</v>
+      </c>
+      <c r="K2319">
+        <v>0</v>
+      </c>
+      <c r="L2319" t="str">
+        <f t="shared" si="103"/>
+        <v>0</v>
+      </c>
+      <c r="M2319" t="str">
+        <f t="shared" si="104"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2320" spans="1:13">
+      <c r="A2320" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="B2320" s="7">
+        <v>173</v>
+      </c>
+      <c r="C2320">
+        <v>8</v>
+      </c>
+      <c r="D2320" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2320">
+        <v>14</v>
+      </c>
+      <c r="F2320" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2320" t="s">
+        <v>568</v>
+      </c>
+      <c r="I2320">
+        <v>1</v>
+      </c>
+      <c r="J2320">
+        <v>2</v>
+      </c>
+      <c r="K2320">
+        <v>0</v>
+      </c>
+      <c r="L2320" t="str">
+        <f t="shared" si="103"/>
+        <v>0</v>
+      </c>
+      <c r="M2320" t="str">
+        <f t="shared" si="104"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2321" spans="1:13">
+      <c r="A2321" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="B2321" s="7">
+        <v>173</v>
+      </c>
+      <c r="C2321">
+        <v>9</v>
+      </c>
+      <c r="D2321" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2321">
+        <v>14</v>
+      </c>
+      <c r="F2321" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2321" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2321">
+        <v>1</v>
+      </c>
+      <c r="J2321">
+        <v>2</v>
+      </c>
+      <c r="K2321">
+        <v>0</v>
+      </c>
+      <c r="L2321" t="str">
+        <f t="shared" si="103"/>
+        <v>0</v>
+      </c>
+      <c r="M2321" t="str">
+        <f t="shared" si="104"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2322" spans="1:13">
+      <c r="A2322" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="B2322" s="7">
+        <v>173</v>
+      </c>
+      <c r="C2322">
+        <v>10</v>
+      </c>
+      <c r="D2322" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2322">
+        <v>14</v>
+      </c>
+      <c r="F2322" t="s">
+        <v>393</v>
+      </c>
+      <c r="G2322" t="s">
+        <v>613</v>
+      </c>
+      <c r="H2322" t="s">
+        <v>612</v>
+      </c>
+      <c r="I2322">
+        <v>0</v>
+      </c>
+      <c r="J2322">
+        <v>3</v>
+      </c>
+      <c r="K2322">
+        <v>0</v>
+      </c>
+      <c r="L2322" t="str">
+        <f t="shared" si="103"/>
+        <v>0</v>
+      </c>
+      <c r="M2322" t="str">
+        <f t="shared" si="104"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new data 2025 12 30
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9405" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9435" uniqueCount="617">
   <si>
     <t>Fecha</t>
   </si>
@@ -1876,6 +1876,15 @@
   <si>
     <t>no de lista</t>
   </si>
+  <si>
+    <t>2025.12.30</t>
+  </si>
+  <si>
+    <t>lista distinta</t>
+  </si>
+  <si>
+    <t>Gruul Stompy</t>
+  </si>
 </sst>
 </file>
 
@@ -2209,13 +2218,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2322"/>
+  <dimension ref="A1:M2329"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2297" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2303" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="G2323" sqref="G2323"/>
+      <selection pane="bottomRight" activeCell="F2329" sqref="F2329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -95489,6 +95498,292 @@
       </c>
       <c r="M2322" t="str">
         <f t="shared" si="104"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2323" spans="1:13">
+      <c r="A2323" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="B2323" s="7">
+        <v>174</v>
+      </c>
+      <c r="C2323">
+        <v>1</v>
+      </c>
+      <c r="D2323" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2323">
+        <v>14</v>
+      </c>
+      <c r="F2323" t="s">
+        <v>236</v>
+      </c>
+      <c r="H2323" t="s">
+        <v>540</v>
+      </c>
+      <c r="I2323">
+        <v>3</v>
+      </c>
+      <c r="J2323">
+        <v>0</v>
+      </c>
+      <c r="K2323">
+        <v>0</v>
+      </c>
+      <c r="L2323" t="str">
+        <f t="shared" ref="L2323:L2329" si="105">IF(C2323=1,"1",IF(C2323=2,"1",IF(C2323=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2323" t="str">
+        <f t="shared" ref="M2323:M2329" si="106">IF(C2323=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2324" spans="1:13">
+      <c r="A2324" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="B2324" s="7">
+        <v>174</v>
+      </c>
+      <c r="C2324">
+        <v>2</v>
+      </c>
+      <c r="D2324" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2324">
+        <v>14</v>
+      </c>
+      <c r="F2324" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2324" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2324">
+        <v>2</v>
+      </c>
+      <c r="J2324">
+        <v>1</v>
+      </c>
+      <c r="K2324">
+        <v>0</v>
+      </c>
+      <c r="L2324" t="str">
+        <f t="shared" si="105"/>
+        <v>1</v>
+      </c>
+      <c r="M2324" t="str">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2325" spans="1:13">
+      <c r="A2325" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="B2325" s="7">
+        <v>174</v>
+      </c>
+      <c r="C2325">
+        <v>3</v>
+      </c>
+      <c r="D2325" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2325">
+        <v>14</v>
+      </c>
+      <c r="F2325" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2325" t="s">
+        <v>615</v>
+      </c>
+      <c r="H2325" t="s">
+        <v>239</v>
+      </c>
+      <c r="I2325">
+        <v>2</v>
+      </c>
+      <c r="J2325">
+        <v>1</v>
+      </c>
+      <c r="K2325">
+        <v>0</v>
+      </c>
+      <c r="L2325" t="str">
+        <f t="shared" si="105"/>
+        <v>1</v>
+      </c>
+      <c r="M2325" t="str">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2326" spans="1:13">
+      <c r="A2326" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="B2326" s="7">
+        <v>174</v>
+      </c>
+      <c r="C2326">
+        <v>4</v>
+      </c>
+      <c r="D2326" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2326">
+        <v>14</v>
+      </c>
+      <c r="F2326" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2326" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2326">
+        <v>2</v>
+      </c>
+      <c r="J2326">
+        <v>1</v>
+      </c>
+      <c r="K2326">
+        <v>0</v>
+      </c>
+      <c r="L2326" t="str">
+        <f t="shared" si="105"/>
+        <v>0</v>
+      </c>
+      <c r="M2326" t="str">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2327" spans="1:13">
+      <c r="A2327" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="B2327" s="7">
+        <v>174</v>
+      </c>
+      <c r="C2327">
+        <v>5</v>
+      </c>
+      <c r="D2327" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2327">
+        <v>14</v>
+      </c>
+      <c r="F2327" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2327" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2327">
+        <v>1</v>
+      </c>
+      <c r="J2327">
+        <v>2</v>
+      </c>
+      <c r="K2327">
+        <v>0</v>
+      </c>
+      <c r="L2327" t="str">
+        <f t="shared" si="105"/>
+        <v>0</v>
+      </c>
+      <c r="M2327" t="str">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2328" spans="1:13">
+      <c r="A2328" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="B2328" s="7">
+        <v>174</v>
+      </c>
+      <c r="C2328">
+        <v>6</v>
+      </c>
+      <c r="D2328" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2328">
+        <v>14</v>
+      </c>
+      <c r="F2328" t="s">
+        <v>616</v>
+      </c>
+      <c r="H2328" t="s">
+        <v>568</v>
+      </c>
+      <c r="I2328">
+        <v>1</v>
+      </c>
+      <c r="J2328">
+        <v>2</v>
+      </c>
+      <c r="K2328">
+        <v>0</v>
+      </c>
+      <c r="L2328" t="str">
+        <f t="shared" si="105"/>
+        <v>0</v>
+      </c>
+      <c r="M2328" t="str">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2329" spans="1:13">
+      <c r="A2329" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="B2329" s="7">
+        <v>174</v>
+      </c>
+      <c r="C2329">
+        <v>7</v>
+      </c>
+      <c r="D2329" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2329">
+        <v>14</v>
+      </c>
+      <c r="F2329" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2329" t="s">
+        <v>533</v>
+      </c>
+      <c r="H2329" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2329">
+        <v>1</v>
+      </c>
+      <c r="J2329">
+        <v>2</v>
+      </c>
+      <c r="K2329">
+        <v>0</v>
+      </c>
+      <c r="L2329" t="str">
+        <f t="shared" si="105"/>
+        <v>0</v>
+      </c>
+      <c r="M2329" t="str">
+        <f t="shared" si="106"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new data 2026 01 02
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9435" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9473" uniqueCount="620">
   <si>
     <t>Fecha</t>
   </si>
@@ -1885,6 +1885,15 @@
   <si>
     <t>Gruul Stompy</t>
   </si>
+  <si>
+    <t>2026.01.02</t>
+  </si>
+  <si>
+    <t>Ene_2026</t>
+  </si>
+  <si>
+    <t>golgari</t>
+  </si>
 </sst>
 </file>
 
@@ -2218,13 +2227,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2329"/>
+  <dimension ref="A1:M2338"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2303" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2318" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F2329" sqref="F2329"/>
+      <selection pane="bottomRight" activeCell="G2339" sqref="G2339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -95784,6 +95793,372 @@
       </c>
       <c r="M2329" t="str">
         <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2330" spans="1:13">
+      <c r="A2330" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="B2330" s="7">
+        <v>175</v>
+      </c>
+      <c r="C2330">
+        <v>1</v>
+      </c>
+      <c r="D2330" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2330">
+        <v>1</v>
+      </c>
+      <c r="F2330" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2330" t="s">
+        <v>619</v>
+      </c>
+      <c r="H2330" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2330">
+        <v>2</v>
+      </c>
+      <c r="J2330">
+        <v>0</v>
+      </c>
+      <c r="K2330">
+        <v>1</v>
+      </c>
+      <c r="L2330" t="str">
+        <f t="shared" ref="L2330:L2338" si="107">IF(C2330=1,"1",IF(C2330=2,"1",IF(C2330=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2330" t="str">
+        <f t="shared" ref="M2330:M2338" si="108">IF(C2330=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2331" spans="1:13">
+      <c r="A2331" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="B2331" s="7">
+        <v>175</v>
+      </c>
+      <c r="C2331">
+        <v>2</v>
+      </c>
+      <c r="D2331" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2331">
+        <v>1</v>
+      </c>
+      <c r="F2331" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2331" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2331">
+        <v>2</v>
+      </c>
+      <c r="J2331">
+        <v>0</v>
+      </c>
+      <c r="K2331">
+        <v>1</v>
+      </c>
+      <c r="L2331" t="str">
+        <f t="shared" si="107"/>
+        <v>1</v>
+      </c>
+      <c r="M2331" t="str">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2332" spans="1:13">
+      <c r="A2332" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="B2332" s="7">
+        <v>175</v>
+      </c>
+      <c r="C2332">
+        <v>3</v>
+      </c>
+      <c r="D2332" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2332">
+        <v>1</v>
+      </c>
+      <c r="F2332" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2332" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2332">
+        <v>2</v>
+      </c>
+      <c r="J2332">
+        <v>0</v>
+      </c>
+      <c r="K2332">
+        <v>1</v>
+      </c>
+      <c r="L2332" t="str">
+        <f t="shared" si="107"/>
+        <v>1</v>
+      </c>
+      <c r="M2332" t="str">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2333" spans="1:13">
+      <c r="A2333" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="B2333" s="7">
+        <v>175</v>
+      </c>
+      <c r="C2333">
+        <v>4</v>
+      </c>
+      <c r="D2333" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2333">
+        <v>1</v>
+      </c>
+      <c r="F2333" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2333" t="s">
+        <v>568</v>
+      </c>
+      <c r="I2333">
+        <v>2</v>
+      </c>
+      <c r="J2333">
+        <v>1</v>
+      </c>
+      <c r="K2333">
+        <v>0</v>
+      </c>
+      <c r="L2333" t="str">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="M2333" t="str">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2334" spans="1:13">
+      <c r="A2334" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="B2334" s="7">
+        <v>175</v>
+      </c>
+      <c r="C2334">
+        <v>5</v>
+      </c>
+      <c r="D2334" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2334">
+        <v>1</v>
+      </c>
+      <c r="F2334" t="s">
+        <v>236</v>
+      </c>
+      <c r="H2334" t="s">
+        <v>540</v>
+      </c>
+      <c r="I2334">
+        <v>2</v>
+      </c>
+      <c r="J2334">
+        <v>1</v>
+      </c>
+      <c r="K2334">
+        <v>0</v>
+      </c>
+      <c r="L2334" t="str">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="M2334" t="str">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2335" spans="1:13">
+      <c r="A2335" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="B2335" s="7">
+        <v>175</v>
+      </c>
+      <c r="C2335">
+        <v>6</v>
+      </c>
+      <c r="D2335" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2335">
+        <v>1</v>
+      </c>
+      <c r="F2335" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2335" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2335">
+        <v>1</v>
+      </c>
+      <c r="J2335">
+        <v>1</v>
+      </c>
+      <c r="K2335">
+        <v>1</v>
+      </c>
+      <c r="L2335" t="str">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="M2335" t="str">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2336" spans="1:13">
+      <c r="A2336" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="B2336" s="7">
+        <v>175</v>
+      </c>
+      <c r="C2336">
+        <v>7</v>
+      </c>
+      <c r="D2336" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2336">
+        <v>1</v>
+      </c>
+      <c r="F2336" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2336" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2336">
+        <v>1</v>
+      </c>
+      <c r="J2336">
+        <v>2</v>
+      </c>
+      <c r="K2336">
+        <v>0</v>
+      </c>
+      <c r="L2336" t="str">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="M2336" t="str">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2337" spans="1:13">
+      <c r="A2337" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="B2337" s="7">
+        <v>175</v>
+      </c>
+      <c r="C2337">
+        <v>8</v>
+      </c>
+      <c r="D2337" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2337">
+        <v>1</v>
+      </c>
+      <c r="F2337" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2337" t="s">
+        <v>416</v>
+      </c>
+      <c r="I2337">
+        <v>0</v>
+      </c>
+      <c r="J2337">
+        <v>2</v>
+      </c>
+      <c r="K2337">
+        <v>0</v>
+      </c>
+      <c r="L2337" t="str">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="M2337" t="str">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2338" spans="1:13">
+      <c r="A2338" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="B2338" s="7">
+        <v>175</v>
+      </c>
+      <c r="C2338">
+        <v>9</v>
+      </c>
+      <c r="D2338" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2338">
+        <v>1</v>
+      </c>
+      <c r="F2338" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2338" t="s">
+        <v>615</v>
+      </c>
+      <c r="H2338" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2338">
+        <v>0</v>
+      </c>
+      <c r="J2338">
+        <v>3</v>
+      </c>
+      <c r="K2338">
+        <v>0</v>
+      </c>
+      <c r="L2338" t="str">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="M2338" t="str">
+        <f t="shared" si="108"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new data 2026 01 03
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9473" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9541" uniqueCount="622">
   <si>
     <t>Fecha</t>
   </si>
@@ -1894,6 +1894,12 @@
   <si>
     <t>golgari</t>
   </si>
+  <si>
+    <t>2026.01.03</t>
+  </si>
+  <si>
+    <t>Boros Gates</t>
+  </si>
 </sst>
 </file>
 
@@ -2227,13 +2233,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2338"/>
+  <dimension ref="A1:M2356"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2318" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B997" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="G2339" sqref="G2339"/>
+      <selection pane="bottomRight" activeCell="F1012" sqref="F1012"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -96159,6 +96165,714 @@
       </c>
       <c r="M2338" t="str">
         <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2339" spans="1:13">
+      <c r="A2339" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2339" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2339">
+        <v>1</v>
+      </c>
+      <c r="D2339" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2339">
+        <v>1</v>
+      </c>
+      <c r="F2339" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2339" t="s">
+        <v>568</v>
+      </c>
+      <c r="I2339">
+        <v>7</v>
+      </c>
+      <c r="J2339">
+        <v>0</v>
+      </c>
+      <c r="K2339">
+        <v>0</v>
+      </c>
+      <c r="L2339" t="str">
+        <f t="shared" ref="L2339:L2356" si="109">IF(C2339=1,"1",IF(C2339=2,"1",IF(C2339=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2339" t="str">
+        <f t="shared" ref="M2339:M2356" si="110">IF(C2339=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2340" spans="1:13">
+      <c r="A2340" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2340" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2340">
+        <v>2</v>
+      </c>
+      <c r="D2340" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2340">
+        <v>1</v>
+      </c>
+      <c r="F2340" t="s">
+        <v>510</v>
+      </c>
+      <c r="H2340" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2340">
+        <v>6</v>
+      </c>
+      <c r="J2340">
+        <v>1</v>
+      </c>
+      <c r="K2340">
+        <v>0</v>
+      </c>
+      <c r="L2340" t="str">
+        <f t="shared" si="109"/>
+        <v>1</v>
+      </c>
+      <c r="M2340" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2341" spans="1:13">
+      <c r="A2341" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2341" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2341">
+        <v>3</v>
+      </c>
+      <c r="D2341" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2341">
+        <v>1</v>
+      </c>
+      <c r="F2341" t="s">
+        <v>510</v>
+      </c>
+      <c r="H2341" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2341">
+        <v>5</v>
+      </c>
+      <c r="J2341">
+        <v>2</v>
+      </c>
+      <c r="K2341">
+        <v>0</v>
+      </c>
+      <c r="L2341" t="str">
+        <f t="shared" si="109"/>
+        <v>1</v>
+      </c>
+      <c r="M2341" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2342" spans="1:13">
+      <c r="A2342" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2342" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2342">
+        <v>4</v>
+      </c>
+      <c r="D2342" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2342">
+        <v>1</v>
+      </c>
+      <c r="F2342" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2342" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2342">
+        <v>5</v>
+      </c>
+      <c r="J2342">
+        <v>2</v>
+      </c>
+      <c r="K2342">
+        <v>0</v>
+      </c>
+      <c r="L2342" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2342" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2343" spans="1:13">
+      <c r="A2343" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2343" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2343">
+        <v>5</v>
+      </c>
+      <c r="D2343" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2343">
+        <v>1</v>
+      </c>
+      <c r="F2343" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2343">
+        <v>0</v>
+      </c>
+      <c r="J2343">
+        <v>0</v>
+      </c>
+      <c r="K2343">
+        <v>0</v>
+      </c>
+      <c r="L2343" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2343" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2344" spans="1:13">
+      <c r="A2344" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2344" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2344">
+        <v>6</v>
+      </c>
+      <c r="D2344" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2344">
+        <v>1</v>
+      </c>
+      <c r="F2344" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2344" t="s">
+        <v>615</v>
+      </c>
+      <c r="H2344" t="s">
+        <v>239</v>
+      </c>
+      <c r="I2344">
+        <v>0</v>
+      </c>
+      <c r="J2344">
+        <v>0</v>
+      </c>
+      <c r="K2344">
+        <v>0</v>
+      </c>
+      <c r="L2344" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2344" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2345" spans="1:13">
+      <c r="A2345" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2345" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2345">
+        <v>7</v>
+      </c>
+      <c r="D2345" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2345">
+        <v>1</v>
+      </c>
+      <c r="F2345" t="s">
+        <v>524</v>
+      </c>
+      <c r="I2345">
+        <v>0</v>
+      </c>
+      <c r="J2345">
+        <v>0</v>
+      </c>
+      <c r="K2345">
+        <v>0</v>
+      </c>
+      <c r="L2345" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2345" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2346" spans="1:13">
+      <c r="A2346" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2346" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2346">
+        <v>8</v>
+      </c>
+      <c r="D2346" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2346">
+        <v>1</v>
+      </c>
+      <c r="F2346" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2346">
+        <v>0</v>
+      </c>
+      <c r="J2346">
+        <v>0</v>
+      </c>
+      <c r="K2346">
+        <v>0</v>
+      </c>
+      <c r="L2346" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2346" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2347" spans="1:13">
+      <c r="A2347" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2347" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2347">
+        <v>9</v>
+      </c>
+      <c r="D2347" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2347">
+        <v>1</v>
+      </c>
+      <c r="F2347" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2347" t="s">
+        <v>544</v>
+      </c>
+      <c r="H2347" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2347">
+        <v>0</v>
+      </c>
+      <c r="J2347">
+        <v>0</v>
+      </c>
+      <c r="K2347">
+        <v>0</v>
+      </c>
+      <c r="L2347" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2347" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2348" spans="1:13">
+      <c r="A2348" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2348" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2348">
+        <v>10</v>
+      </c>
+      <c r="D2348" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2348">
+        <v>1</v>
+      </c>
+      <c r="F2348" t="s">
+        <v>393</v>
+      </c>
+      <c r="H2348" t="s">
+        <v>301</v>
+      </c>
+      <c r="I2348">
+        <v>0</v>
+      </c>
+      <c r="J2348">
+        <v>0</v>
+      </c>
+      <c r="K2348">
+        <v>0</v>
+      </c>
+      <c r="L2348" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2348" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2349" spans="1:13">
+      <c r="A2349" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2349" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2349">
+        <v>11</v>
+      </c>
+      <c r="D2349" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2349">
+        <v>1</v>
+      </c>
+      <c r="F2349" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2349">
+        <v>0</v>
+      </c>
+      <c r="J2349">
+        <v>0</v>
+      </c>
+      <c r="K2349">
+        <v>0</v>
+      </c>
+      <c r="L2349" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2349" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2350" spans="1:13">
+      <c r="A2350" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2350" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2350">
+        <v>12</v>
+      </c>
+      <c r="D2350" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2350">
+        <v>1</v>
+      </c>
+      <c r="F2350" t="s">
+        <v>377</v>
+      </c>
+      <c r="I2350">
+        <v>0</v>
+      </c>
+      <c r="J2350">
+        <v>0</v>
+      </c>
+      <c r="K2350">
+        <v>0</v>
+      </c>
+      <c r="L2350" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2350" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2351" spans="1:13">
+      <c r="A2351" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2351" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2351">
+        <v>13</v>
+      </c>
+      <c r="D2351" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2351">
+        <v>1</v>
+      </c>
+      <c r="F2351" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2351" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2351">
+        <v>0</v>
+      </c>
+      <c r="J2351">
+        <v>0</v>
+      </c>
+      <c r="K2351">
+        <v>0</v>
+      </c>
+      <c r="L2351" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2351" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2352" spans="1:13">
+      <c r="A2352" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2352" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2352">
+        <v>14</v>
+      </c>
+      <c r="D2352" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2352">
+        <v>1</v>
+      </c>
+      <c r="F2352" t="s">
+        <v>571</v>
+      </c>
+      <c r="H2352" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2352">
+        <v>0</v>
+      </c>
+      <c r="J2352">
+        <v>0</v>
+      </c>
+      <c r="K2352">
+        <v>0</v>
+      </c>
+      <c r="L2352" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2352" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2353" spans="1:13">
+      <c r="A2353" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2353" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2353">
+        <v>15</v>
+      </c>
+      <c r="D2353" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2353">
+        <v>1</v>
+      </c>
+      <c r="F2353" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2353" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2353">
+        <v>0</v>
+      </c>
+      <c r="J2353">
+        <v>0</v>
+      </c>
+      <c r="K2353">
+        <v>0</v>
+      </c>
+      <c r="L2353" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2353" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2354" spans="1:13">
+      <c r="A2354" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2354" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2354">
+        <v>16</v>
+      </c>
+      <c r="D2354" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2354">
+        <v>1</v>
+      </c>
+      <c r="F2354" t="s">
+        <v>551</v>
+      </c>
+      <c r="H2354" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2354">
+        <v>0</v>
+      </c>
+      <c r="J2354">
+        <v>0</v>
+      </c>
+      <c r="K2354">
+        <v>0</v>
+      </c>
+      <c r="L2354" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2354" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2355" spans="1:13">
+      <c r="A2355" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2355" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2355">
+        <v>17</v>
+      </c>
+      <c r="D2355" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2355">
+        <v>1</v>
+      </c>
+      <c r="F2355" t="s">
+        <v>621</v>
+      </c>
+      <c r="I2355">
+        <v>0</v>
+      </c>
+      <c r="J2355">
+        <v>0</v>
+      </c>
+      <c r="K2355">
+        <v>0</v>
+      </c>
+      <c r="L2355" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2355" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2356" spans="1:13">
+      <c r="A2356" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2356" s="7">
+        <v>176</v>
+      </c>
+      <c r="C2356">
+        <v>18</v>
+      </c>
+      <c r="D2356" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2356">
+        <v>1</v>
+      </c>
+      <c r="F2356" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2356" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2356">
+        <v>0</v>
+      </c>
+      <c r="J2356">
+        <v>0</v>
+      </c>
+      <c r="K2356">
+        <v>0</v>
+      </c>
+      <c r="L2356" t="str">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="M2356" t="str">
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data 2026 01 03 changed
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -2236,10 +2236,10 @@
   <dimension ref="A1:M2356"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B997" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2330" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F1012" sqref="F1012"/>
+      <selection pane="bottomRight" activeCell="I2343" sqref="I2343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -96191,7 +96191,7 @@
         <v>568</v>
       </c>
       <c r="I2339">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J2339">
         <v>0</v>
@@ -96231,7 +96231,7 @@
         <v>34</v>
       </c>
       <c r="I2340">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J2340">
         <v>1</v>
@@ -96271,7 +96271,7 @@
         <v>74</v>
       </c>
       <c r="I2341">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J2341">
         <v>2</v>
@@ -96308,10 +96308,10 @@
         <v>31</v>
       </c>
       <c r="H2342" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I2342">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J2342">
         <v>2</v>
@@ -96656,10 +96656,10 @@
         <v>1</v>
       </c>
       <c r="F2351" t="s">
-        <v>31</v>
+        <v>524</v>
       </c>
       <c r="H2351" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I2351">
         <v>0</v>

</xml_diff>

<commit_message>
new data 2026 01 09 and 2026 01 16
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9541" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9585" uniqueCount="624">
   <si>
     <t>Fecha</t>
   </si>
@@ -1900,6 +1900,12 @@
   <si>
     <t>Boros Gates</t>
   </si>
+  <si>
+    <t>2026.01.09</t>
+  </si>
+  <si>
+    <t>2026.01.16</t>
+  </si>
 </sst>
 </file>
 
@@ -2233,13 +2239,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2356"/>
+  <dimension ref="A1:M2367"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2330" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2351" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="I2343" sqref="I2343"/>
+      <selection pane="bottomRight" activeCell="F2372" sqref="F2372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -96873,6 +96879,446 @@
       </c>
       <c r="M2356" t="str">
         <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2357" spans="1:13">
+      <c r="A2357" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="B2357" s="7">
+        <v>177</v>
+      </c>
+      <c r="C2357">
+        <v>1</v>
+      </c>
+      <c r="D2357" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2357">
+        <v>1</v>
+      </c>
+      <c r="F2357" t="s">
+        <v>571</v>
+      </c>
+      <c r="H2357" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2357">
+        <v>3</v>
+      </c>
+      <c r="J2357">
+        <v>0</v>
+      </c>
+      <c r="K2357">
+        <v>0</v>
+      </c>
+      <c r="L2357" t="str">
+        <f t="shared" ref="L2357:L2367" si="111">IF(C2357=1,"1",IF(C2357=2,"1",IF(C2357=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2357" t="str">
+        <f t="shared" ref="M2357:M2367" si="112">IF(C2357=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2358" spans="1:13">
+      <c r="A2358" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="B2358" s="7">
+        <v>177</v>
+      </c>
+      <c r="C2358">
+        <v>2</v>
+      </c>
+      <c r="D2358" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2358">
+        <v>1</v>
+      </c>
+      <c r="F2358" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2358" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2358">
+        <v>2</v>
+      </c>
+      <c r="J2358">
+        <v>1</v>
+      </c>
+      <c r="K2358">
+        <v>0</v>
+      </c>
+      <c r="L2358" t="str">
+        <f t="shared" si="111"/>
+        <v>1</v>
+      </c>
+      <c r="M2358" t="str">
+        <f t="shared" si="112"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2359" spans="1:13">
+      <c r="A2359" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="B2359" s="7">
+        <v>177</v>
+      </c>
+      <c r="C2359">
+        <v>3</v>
+      </c>
+      <c r="D2359" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2359">
+        <v>1</v>
+      </c>
+      <c r="F2359" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2359" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2359">
+        <v>2</v>
+      </c>
+      <c r="J2359">
+        <v>1</v>
+      </c>
+      <c r="K2359">
+        <v>0</v>
+      </c>
+      <c r="L2359" t="str">
+        <f t="shared" si="111"/>
+        <v>1</v>
+      </c>
+      <c r="M2359" t="str">
+        <f t="shared" si="112"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2360" spans="1:13">
+      <c r="A2360" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="B2360" s="7">
+        <v>177</v>
+      </c>
+      <c r="C2360">
+        <v>4</v>
+      </c>
+      <c r="D2360" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2360">
+        <v>1</v>
+      </c>
+      <c r="F2360" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2360" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2360">
+        <v>2</v>
+      </c>
+      <c r="J2360">
+        <v>1</v>
+      </c>
+      <c r="K2360">
+        <v>0</v>
+      </c>
+      <c r="L2360" t="str">
+        <f t="shared" si="111"/>
+        <v>0</v>
+      </c>
+      <c r="M2360" t="str">
+        <f t="shared" si="112"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2361" spans="1:13">
+      <c r="A2361" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="B2361" s="7">
+        <v>177</v>
+      </c>
+      <c r="C2361">
+        <v>5</v>
+      </c>
+      <c r="D2361" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2361">
+        <v>1</v>
+      </c>
+      <c r="F2361" t="s">
+        <v>163</v>
+      </c>
+      <c r="H2361" t="s">
+        <v>451</v>
+      </c>
+      <c r="I2361">
+        <v>1</v>
+      </c>
+      <c r="J2361">
+        <v>2</v>
+      </c>
+      <c r="K2361">
+        <v>0</v>
+      </c>
+      <c r="L2361" t="str">
+        <f t="shared" si="111"/>
+        <v>0</v>
+      </c>
+      <c r="M2361" t="str">
+        <f t="shared" si="112"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2362" spans="1:13">
+      <c r="A2362" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="B2362" s="7">
+        <v>177</v>
+      </c>
+      <c r="C2362">
+        <v>6</v>
+      </c>
+      <c r="D2362" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2362">
+        <v>1</v>
+      </c>
+      <c r="F2362" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2362" t="s">
+        <v>568</v>
+      </c>
+      <c r="I2362">
+        <v>1</v>
+      </c>
+      <c r="J2362">
+        <v>2</v>
+      </c>
+      <c r="K2362">
+        <v>0</v>
+      </c>
+      <c r="L2362" t="str">
+        <f t="shared" si="111"/>
+        <v>0</v>
+      </c>
+      <c r="M2362" t="str">
+        <f t="shared" si="112"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2363" spans="1:13">
+      <c r="A2363" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="B2363" s="7">
+        <v>177</v>
+      </c>
+      <c r="C2363">
+        <v>7</v>
+      </c>
+      <c r="D2363" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2363">
+        <v>1</v>
+      </c>
+      <c r="F2363" t="s">
+        <v>236</v>
+      </c>
+      <c r="H2363" t="s">
+        <v>540</v>
+      </c>
+      <c r="I2363">
+        <v>1</v>
+      </c>
+      <c r="J2363">
+        <v>2</v>
+      </c>
+      <c r="K2363">
+        <v>0</v>
+      </c>
+      <c r="L2363" t="str">
+        <f t="shared" si="111"/>
+        <v>0</v>
+      </c>
+      <c r="M2363" t="str">
+        <f t="shared" si="112"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2364" spans="1:13">
+      <c r="A2364" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="B2364" s="7">
+        <v>178</v>
+      </c>
+      <c r="C2364">
+        <v>1</v>
+      </c>
+      <c r="D2364" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2364">
+        <v>1</v>
+      </c>
+      <c r="F2364" t="s">
+        <v>551</v>
+      </c>
+      <c r="H2364" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2364">
+        <v>3</v>
+      </c>
+      <c r="J2364">
+        <v>0</v>
+      </c>
+      <c r="K2364">
+        <v>0</v>
+      </c>
+      <c r="L2364" t="str">
+        <f t="shared" si="111"/>
+        <v>1</v>
+      </c>
+      <c r="M2364" t="str">
+        <f t="shared" si="112"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2365" spans="1:13">
+      <c r="A2365" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="B2365" s="7">
+        <v>178</v>
+      </c>
+      <c r="C2365">
+        <v>2</v>
+      </c>
+      <c r="D2365" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2365">
+        <v>1</v>
+      </c>
+      <c r="F2365" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2365" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2365">
+        <v>2</v>
+      </c>
+      <c r="J2365">
+        <v>1</v>
+      </c>
+      <c r="K2365">
+        <v>0</v>
+      </c>
+      <c r="L2365" t="str">
+        <f t="shared" si="111"/>
+        <v>1</v>
+      </c>
+      <c r="M2365" t="str">
+        <f t="shared" si="112"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2366" spans="1:13">
+      <c r="A2366" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="B2366" s="7">
+        <v>178</v>
+      </c>
+      <c r="C2366">
+        <v>3</v>
+      </c>
+      <c r="D2366" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2366">
+        <v>1</v>
+      </c>
+      <c r="F2366" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2366" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2366">
+        <v>1</v>
+      </c>
+      <c r="J2366">
+        <v>2</v>
+      </c>
+      <c r="K2366">
+        <v>0</v>
+      </c>
+      <c r="L2366" t="str">
+        <f t="shared" si="111"/>
+        <v>1</v>
+      </c>
+      <c r="M2366" t="str">
+        <f t="shared" si="112"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2367" spans="1:13">
+      <c r="A2367" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="B2367" s="7">
+        <v>178</v>
+      </c>
+      <c r="C2367">
+        <v>4</v>
+      </c>
+      <c r="D2367" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2367">
+        <v>1</v>
+      </c>
+      <c r="F2367" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2367" t="s">
+        <v>612</v>
+      </c>
+      <c r="I2367">
+        <v>0</v>
+      </c>
+      <c r="J2367">
+        <v>3</v>
+      </c>
+      <c r="K2367">
+        <v>0</v>
+      </c>
+      <c r="L2367" t="str">
+        <f t="shared" si="111"/>
+        <v>0</v>
+      </c>
+      <c r="M2367" t="str">
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new data 2026 01 20
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9585" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9644" uniqueCount="628">
   <si>
     <t>Fecha</t>
   </si>
@@ -1906,6 +1906,18 @@
   <si>
     <t>2026.01.16</t>
   </si>
+  <si>
+    <t>2026.01.20</t>
+  </si>
+  <si>
+    <t>jose moya</t>
+  </si>
+  <si>
+    <t>mono red</t>
+  </si>
+  <si>
+    <t>splash black</t>
+  </si>
 </sst>
 </file>
 
@@ -2239,13 +2251,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2367"/>
+  <dimension ref="A1:M2381"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2351" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2357" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F2372" sqref="F2372"/>
+      <selection pane="bottomRight" activeCell="F2382" sqref="F2382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -97301,6 +97313,9 @@
       <c r="F2367" t="s">
         <v>26</v>
       </c>
+      <c r="G2367" t="s">
+        <v>627</v>
+      </c>
       <c r="H2367" t="s">
         <v>612</v>
       </c>
@@ -97319,6 +97334,572 @@
       </c>
       <c r="M2367" t="str">
         <f t="shared" si="112"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2368" spans="1:13">
+      <c r="A2368" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2368" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2368">
+        <v>1</v>
+      </c>
+      <c r="D2368" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2368">
+        <v>1</v>
+      </c>
+      <c r="F2368" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2368" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2368">
+        <v>2</v>
+      </c>
+      <c r="J2368">
+        <v>0</v>
+      </c>
+      <c r="K2368">
+        <v>1</v>
+      </c>
+      <c r="L2368" t="str">
+        <f t="shared" ref="L2368:L2381" si="113">IF(C2368=1,"1",IF(C2368=2,"1",IF(C2368=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2368" t="str">
+        <f t="shared" ref="M2368:M2381" si="114">IF(C2368=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2369" spans="1:13">
+      <c r="A2369" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2369" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2369">
+        <v>2</v>
+      </c>
+      <c r="D2369" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2369">
+        <v>1</v>
+      </c>
+      <c r="F2369" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2369" t="s">
+        <v>626</v>
+      </c>
+      <c r="H2369" t="s">
+        <v>625</v>
+      </c>
+      <c r="I2369">
+        <v>2</v>
+      </c>
+      <c r="J2369">
+        <v>0</v>
+      </c>
+      <c r="K2369">
+        <v>1</v>
+      </c>
+      <c r="L2369" t="str">
+        <f t="shared" si="113"/>
+        <v>1</v>
+      </c>
+      <c r="M2369" t="str">
+        <f t="shared" si="114"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2370" spans="1:13">
+      <c r="A2370" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2370" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2370">
+        <v>3</v>
+      </c>
+      <c r="D2370" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2370">
+        <v>1</v>
+      </c>
+      <c r="F2370" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2370" t="s">
+        <v>423</v>
+      </c>
+      <c r="I2370">
+        <v>2</v>
+      </c>
+      <c r="J2370">
+        <v>0</v>
+      </c>
+      <c r="K2370">
+        <v>1</v>
+      </c>
+      <c r="L2370" t="str">
+        <f t="shared" si="113"/>
+        <v>1</v>
+      </c>
+      <c r="M2370" t="str">
+        <f t="shared" si="114"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2371" spans="1:13">
+      <c r="A2371" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2371" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2371">
+        <v>4</v>
+      </c>
+      <c r="D2371" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2371">
+        <v>1</v>
+      </c>
+      <c r="F2371" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2371" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2371">
+        <v>2</v>
+      </c>
+      <c r="J2371">
+        <v>1</v>
+      </c>
+      <c r="K2371">
+        <v>0</v>
+      </c>
+      <c r="L2371" t="str">
+        <f t="shared" si="113"/>
+        <v>0</v>
+      </c>
+      <c r="M2371" t="str">
+        <f t="shared" si="114"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2372" spans="1:13">
+      <c r="A2372" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2372" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2372">
+        <v>5</v>
+      </c>
+      <c r="D2372" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2372">
+        <v>1</v>
+      </c>
+      <c r="F2372" t="s">
+        <v>571</v>
+      </c>
+      <c r="H2372" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2372">
+        <v>2</v>
+      </c>
+      <c r="J2372">
+        <v>1</v>
+      </c>
+      <c r="K2372">
+        <v>0</v>
+      </c>
+      <c r="L2372" t="str">
+        <f t="shared" si="113"/>
+        <v>0</v>
+      </c>
+      <c r="M2372" t="str">
+        <f t="shared" si="114"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2373" spans="1:13">
+      <c r="A2373" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2373" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2373">
+        <v>6</v>
+      </c>
+      <c r="D2373" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2373">
+        <v>1</v>
+      </c>
+      <c r="F2373" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2373" t="s">
+        <v>568</v>
+      </c>
+      <c r="I2373">
+        <v>2</v>
+      </c>
+      <c r="J2373">
+        <v>1</v>
+      </c>
+      <c r="K2373">
+        <v>0</v>
+      </c>
+      <c r="L2373" t="str">
+        <f t="shared" si="113"/>
+        <v>0</v>
+      </c>
+      <c r="M2373" t="str">
+        <f t="shared" si="114"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2374" spans="1:13">
+      <c r="A2374" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2374" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2374">
+        <v>7</v>
+      </c>
+      <c r="D2374" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2374">
+        <v>1</v>
+      </c>
+      <c r="F2374" t="s">
+        <v>572</v>
+      </c>
+      <c r="H2374" t="s">
+        <v>540</v>
+      </c>
+      <c r="I2374">
+        <v>1</v>
+      </c>
+      <c r="J2374">
+        <v>0</v>
+      </c>
+      <c r="K2374">
+        <v>2</v>
+      </c>
+      <c r="L2374" t="str">
+        <f t="shared" si="113"/>
+        <v>0</v>
+      </c>
+      <c r="M2374" t="str">
+        <f t="shared" si="114"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2375" spans="1:13">
+      <c r="A2375" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2375" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2375">
+        <v>8</v>
+      </c>
+      <c r="D2375" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2375">
+        <v>1</v>
+      </c>
+      <c r="F2375" t="s">
+        <v>396</v>
+      </c>
+      <c r="H2375" t="s">
+        <v>578</v>
+      </c>
+      <c r="I2375">
+        <v>1</v>
+      </c>
+      <c r="J2375">
+        <v>1</v>
+      </c>
+      <c r="K2375">
+        <v>1</v>
+      </c>
+      <c r="L2375" t="str">
+        <f t="shared" si="113"/>
+        <v>0</v>
+      </c>
+      <c r="M2375" t="str">
+        <f t="shared" si="114"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2376" spans="1:13">
+      <c r="A2376" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2376" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2376">
+        <v>9</v>
+      </c>
+      <c r="D2376" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2376">
+        <v>1</v>
+      </c>
+      <c r="F2376" t="s">
+        <v>217</v>
+      </c>
+      <c r="H2376" t="s">
+        <v>201</v>
+      </c>
+      <c r="I2376">
+        <v>1</v>
+      </c>
+      <c r="J2376">
+        <v>2</v>
+      </c>
+      <c r="K2376">
+        <v>0</v>
+      </c>
+      <c r="L2376" t="str">
+        <f t="shared" si="113"/>
+        <v>0</v>
+      </c>
+      <c r="M2376" t="str">
+        <f t="shared" si="114"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2377" spans="1:13">
+      <c r="A2377" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2377" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2377">
+        <v>10</v>
+      </c>
+      <c r="D2377" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2377">
+        <v>1</v>
+      </c>
+      <c r="F2377" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2377" t="s">
+        <v>627</v>
+      </c>
+      <c r="H2377" t="s">
+        <v>612</v>
+      </c>
+      <c r="I2377">
+        <v>1</v>
+      </c>
+      <c r="J2377">
+        <v>2</v>
+      </c>
+      <c r="K2377">
+        <v>0</v>
+      </c>
+      <c r="L2377" t="str">
+        <f t="shared" si="113"/>
+        <v>0</v>
+      </c>
+      <c r="M2377" t="str">
+        <f t="shared" si="114"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2378" spans="1:13">
+      <c r="A2378" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2378" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2378">
+        <v>11</v>
+      </c>
+      <c r="D2378" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2378">
+        <v>1</v>
+      </c>
+      <c r="F2378" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2378" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2378">
+        <v>1</v>
+      </c>
+      <c r="J2378">
+        <v>2</v>
+      </c>
+      <c r="K2378">
+        <v>0</v>
+      </c>
+      <c r="L2378" t="str">
+        <f t="shared" si="113"/>
+        <v>0</v>
+      </c>
+      <c r="M2378" t="str">
+        <f t="shared" si="114"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2379" spans="1:13">
+      <c r="A2379" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2379" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2379">
+        <v>12</v>
+      </c>
+      <c r="D2379" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2379">
+        <v>1</v>
+      </c>
+      <c r="F2379" t="s">
+        <v>396</v>
+      </c>
+      <c r="H2379" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2379">
+        <v>1</v>
+      </c>
+      <c r="J2379">
+        <v>2</v>
+      </c>
+      <c r="K2379">
+        <v>0</v>
+      </c>
+      <c r="L2379" t="str">
+        <f t="shared" si="113"/>
+        <v>0</v>
+      </c>
+      <c r="M2379" t="str">
+        <f t="shared" si="114"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2380" spans="1:13">
+      <c r="A2380" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2380" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2380">
+        <v>13</v>
+      </c>
+      <c r="D2380" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2380">
+        <v>1</v>
+      </c>
+      <c r="F2380" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2380" t="s">
+        <v>581</v>
+      </c>
+      <c r="I2380">
+        <v>0</v>
+      </c>
+      <c r="J2380">
+        <v>3</v>
+      </c>
+      <c r="K2380">
+        <v>0</v>
+      </c>
+      <c r="L2380" t="str">
+        <f t="shared" si="113"/>
+        <v>0</v>
+      </c>
+      <c r="M2380" t="str">
+        <f t="shared" si="114"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2381" spans="1:13">
+      <c r="A2381" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2381" s="7">
+        <v>179</v>
+      </c>
+      <c r="C2381">
+        <v>14</v>
+      </c>
+      <c r="D2381" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2381">
+        <v>1</v>
+      </c>
+      <c r="F2381" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2381" t="s">
+        <v>483</v>
+      </c>
+      <c r="I2381">
+        <v>0</v>
+      </c>
+      <c r="J2381">
+        <v>3</v>
+      </c>
+      <c r="K2381">
+        <v>0</v>
+      </c>
+      <c r="L2381" t="str">
+        <f t="shared" si="113"/>
+        <v>0</v>
+      </c>
+      <c r="M2381" t="str">
+        <f t="shared" si="114"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new data 2026 01 26
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9644" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9693" uniqueCount="629">
   <si>
     <t>Fecha</t>
   </si>
@@ -1918,6 +1918,9 @@
   <si>
     <t>splash black</t>
   </si>
+  <si>
+    <t>2026.01.27</t>
+  </si>
 </sst>
 </file>
 
@@ -2251,13 +2254,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2381"/>
+  <dimension ref="A1:M2393"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2357" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2366" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F2382" sqref="F2382"/>
+      <selection pane="bottomRight" activeCell="F2391" sqref="F2391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -97900,6 +97903,489 @@
       </c>
       <c r="M2381" t="str">
         <f t="shared" si="114"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2382" spans="1:13">
+      <c r="A2382" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2382" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2382">
+        <v>1</v>
+      </c>
+      <c r="D2382" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2382">
+        <v>1</v>
+      </c>
+      <c r="F2382" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2382" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2382">
+        <v>3</v>
+      </c>
+      <c r="J2382">
+        <v>0</v>
+      </c>
+      <c r="K2382">
+        <v>0</v>
+      </c>
+      <c r="L2382" t="str">
+        <f t="shared" ref="L2382:L2393" si="115">IF(C2382=1,"1",IF(C2382=2,"1",IF(C2382=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2382" t="str">
+        <f t="shared" ref="M2382:M2393" si="116">IF(C2382=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2383" spans="1:13">
+      <c r="A2383" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2383" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2383">
+        <v>2</v>
+      </c>
+      <c r="D2383" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2383">
+        <v>1</v>
+      </c>
+      <c r="F2383" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2383" t="s">
+        <v>626</v>
+      </c>
+      <c r="H2383" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2383">
+        <v>3</v>
+      </c>
+      <c r="J2383">
+        <v>0</v>
+      </c>
+      <c r="K2383">
+        <v>0</v>
+      </c>
+      <c r="L2383" t="str">
+        <f t="shared" si="115"/>
+        <v>1</v>
+      </c>
+      <c r="M2383" t="str">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2384" spans="1:13">
+      <c r="A2384" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2384" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2384">
+        <v>3</v>
+      </c>
+      <c r="D2384" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2384">
+        <v>1</v>
+      </c>
+      <c r="F2384" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2384" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2384">
+        <v>2</v>
+      </c>
+      <c r="J2384">
+        <v>1</v>
+      </c>
+      <c r="K2384">
+        <v>0</v>
+      </c>
+      <c r="L2384" t="str">
+        <f t="shared" si="115"/>
+        <v>1</v>
+      </c>
+      <c r="M2384" t="str">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2385" spans="1:13">
+      <c r="A2385" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2385" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2385">
+        <v>4</v>
+      </c>
+      <c r="D2385" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2385">
+        <v>1</v>
+      </c>
+      <c r="F2385" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2385" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2385">
+        <v>2</v>
+      </c>
+      <c r="J2385">
+        <v>1</v>
+      </c>
+      <c r="K2385">
+        <v>0</v>
+      </c>
+      <c r="L2385" t="str">
+        <f t="shared" si="115"/>
+        <v>0</v>
+      </c>
+      <c r="M2385" t="str">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2386" spans="1:13">
+      <c r="A2386" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2386" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2386">
+        <v>5</v>
+      </c>
+      <c r="D2386" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2386">
+        <v>1</v>
+      </c>
+      <c r="F2386" t="s">
+        <v>551</v>
+      </c>
+      <c r="H2386" t="s">
+        <v>416</v>
+      </c>
+      <c r="I2386">
+        <v>2</v>
+      </c>
+      <c r="J2386">
+        <v>1</v>
+      </c>
+      <c r="K2386">
+        <v>0</v>
+      </c>
+      <c r="L2386" t="str">
+        <f t="shared" si="115"/>
+        <v>0</v>
+      </c>
+      <c r="M2386" t="str">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2387" spans="1:13">
+      <c r="A2387" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2387" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2387">
+        <v>6</v>
+      </c>
+      <c r="D2387" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2387">
+        <v>1</v>
+      </c>
+      <c r="F2387" t="s">
+        <v>396</v>
+      </c>
+      <c r="H2387" t="s">
+        <v>201</v>
+      </c>
+      <c r="I2387">
+        <v>1</v>
+      </c>
+      <c r="J2387">
+        <v>2</v>
+      </c>
+      <c r="K2387">
+        <v>0</v>
+      </c>
+      <c r="L2387" t="str">
+        <f t="shared" si="115"/>
+        <v>0</v>
+      </c>
+      <c r="M2387" t="str">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2388" spans="1:13">
+      <c r="A2388" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2388" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2388">
+        <v>7</v>
+      </c>
+      <c r="D2388" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2388">
+        <v>1</v>
+      </c>
+      <c r="F2388" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2388" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2388">
+        <v>1</v>
+      </c>
+      <c r="J2388">
+        <v>2</v>
+      </c>
+      <c r="K2388">
+        <v>0</v>
+      </c>
+      <c r="L2388" t="str">
+        <f t="shared" si="115"/>
+        <v>0</v>
+      </c>
+      <c r="M2388" t="str">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:13">
+      <c r="A2389" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2389" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2389">
+        <v>8</v>
+      </c>
+      <c r="D2389" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2389">
+        <v>1</v>
+      </c>
+      <c r="F2389" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2389" t="s">
+        <v>578</v>
+      </c>
+      <c r="I2389">
+        <v>1</v>
+      </c>
+      <c r="J2389">
+        <v>2</v>
+      </c>
+      <c r="K2389">
+        <v>0</v>
+      </c>
+      <c r="L2389" t="str">
+        <f t="shared" si="115"/>
+        <v>0</v>
+      </c>
+      <c r="M2389" t="str">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:13">
+      <c r="A2390" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2390" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2390">
+        <v>9</v>
+      </c>
+      <c r="D2390" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2390">
+        <v>1</v>
+      </c>
+      <c r="F2390" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2390" t="s">
+        <v>189</v>
+      </c>
+      <c r="I2390">
+        <v>1</v>
+      </c>
+      <c r="J2390">
+        <v>2</v>
+      </c>
+      <c r="K2390">
+        <v>0</v>
+      </c>
+      <c r="L2390" t="str">
+        <f t="shared" si="115"/>
+        <v>0</v>
+      </c>
+      <c r="M2390" t="str">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:13">
+      <c r="A2391" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2391" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2391">
+        <v>10</v>
+      </c>
+      <c r="D2391" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2391">
+        <v>1</v>
+      </c>
+      <c r="F2391" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2391" t="s">
+        <v>593</v>
+      </c>
+      <c r="I2391">
+        <v>1</v>
+      </c>
+      <c r="J2391">
+        <v>2</v>
+      </c>
+      <c r="K2391">
+        <v>0</v>
+      </c>
+      <c r="L2391" t="str">
+        <f t="shared" si="115"/>
+        <v>0</v>
+      </c>
+      <c r="M2391" t="str">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:13">
+      <c r="A2392" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2392" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2392">
+        <v>11</v>
+      </c>
+      <c r="D2392" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2392">
+        <v>1</v>
+      </c>
+      <c r="F2392" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2392" t="s">
+        <v>568</v>
+      </c>
+      <c r="I2392">
+        <v>1</v>
+      </c>
+      <c r="J2392">
+        <v>2</v>
+      </c>
+      <c r="K2392">
+        <v>0</v>
+      </c>
+      <c r="L2392" t="str">
+        <f t="shared" si="115"/>
+        <v>0</v>
+      </c>
+      <c r="M2392" t="str">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2393" spans="1:13">
+      <c r="A2393" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2393" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2393">
+        <v>12</v>
+      </c>
+      <c r="D2393" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2393">
+        <v>1</v>
+      </c>
+      <c r="F2393" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2393" t="s">
+        <v>612</v>
+      </c>
+      <c r="I2393">
+        <v>1</v>
+      </c>
+      <c r="J2393">
+        <v>2</v>
+      </c>
+      <c r="K2393">
+        <v>0</v>
+      </c>
+      <c r="L2393" t="str">
+        <f t="shared" si="115"/>
+        <v>0</v>
+      </c>
+      <c r="M2393" t="str">
+        <f t="shared" si="116"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new data 2026 02 03
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9693" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9742" uniqueCount="632">
   <si>
     <t>Fecha</t>
   </si>
@@ -1921,6 +1921,15 @@
   <si>
     <t>2026.01.27</t>
   </si>
+  <si>
+    <t>2026.02.03</t>
+  </si>
+  <si>
+    <t>Feb_2026</t>
+  </si>
+  <si>
+    <t>monster</t>
+  </si>
 </sst>
 </file>
 
@@ -2254,13 +2263,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2393"/>
+  <dimension ref="A1:M2405"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2366" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2384" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F2391" sqref="F2391"/>
+      <selection pane="bottomRight" activeCell="F2406" sqref="F2406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -98386,6 +98395,489 @@
       </c>
       <c r="M2393" t="str">
         <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:13">
+      <c r="A2394" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2394" s="7">
+        <v>181</v>
+      </c>
+      <c r="C2394">
+        <v>1</v>
+      </c>
+      <c r="D2394" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2394">
+        <v>1</v>
+      </c>
+      <c r="F2394" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2394" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2394">
+        <v>3</v>
+      </c>
+      <c r="J2394">
+        <v>0</v>
+      </c>
+      <c r="K2394">
+        <v>0</v>
+      </c>
+      <c r="L2394" t="str">
+        <f t="shared" ref="L2394:L2405" si="117">IF(C2394=1,"1",IF(C2394=2,"1",IF(C2394=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2394" t="str">
+        <f t="shared" ref="M2394:M2405" si="118">IF(C2394=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:13">
+      <c r="A2395" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2395" s="7">
+        <v>181</v>
+      </c>
+      <c r="C2395">
+        <v>2</v>
+      </c>
+      <c r="D2395" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2395">
+        <v>1</v>
+      </c>
+      <c r="F2395" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2395" t="s">
+        <v>578</v>
+      </c>
+      <c r="I2395">
+        <v>3</v>
+      </c>
+      <c r="J2395">
+        <v>0</v>
+      </c>
+      <c r="K2395">
+        <v>0</v>
+      </c>
+      <c r="L2395" t="str">
+        <f t="shared" si="117"/>
+        <v>1</v>
+      </c>
+      <c r="M2395" t="str">
+        <f t="shared" si="118"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:13">
+      <c r="A2396" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2396" s="7">
+        <v>181</v>
+      </c>
+      <c r="C2396">
+        <v>3</v>
+      </c>
+      <c r="D2396" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2396">
+        <v>1</v>
+      </c>
+      <c r="F2396" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2396" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2396">
+        <v>2</v>
+      </c>
+      <c r="J2396">
+        <v>1</v>
+      </c>
+      <c r="K2396">
+        <v>0</v>
+      </c>
+      <c r="L2396" t="str">
+        <f t="shared" si="117"/>
+        <v>1</v>
+      </c>
+      <c r="M2396" t="str">
+        <f t="shared" si="118"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:13">
+      <c r="A2397" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2397" s="7">
+        <v>181</v>
+      </c>
+      <c r="C2397">
+        <v>4</v>
+      </c>
+      <c r="D2397" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2397">
+        <v>1</v>
+      </c>
+      <c r="F2397" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2397" t="s">
+        <v>631</v>
+      </c>
+      <c r="H2397" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2397">
+        <v>2</v>
+      </c>
+      <c r="J2397">
+        <v>1</v>
+      </c>
+      <c r="K2397">
+        <v>0</v>
+      </c>
+      <c r="L2397" t="str">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="M2397" t="str">
+        <f t="shared" si="118"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:13">
+      <c r="A2398" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2398" s="7">
+        <v>181</v>
+      </c>
+      <c r="C2398">
+        <v>5</v>
+      </c>
+      <c r="D2398" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2398">
+        <v>1</v>
+      </c>
+      <c r="F2398" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2398" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2398">
+        <v>2</v>
+      </c>
+      <c r="J2398">
+        <v>1</v>
+      </c>
+      <c r="K2398">
+        <v>0</v>
+      </c>
+      <c r="L2398" t="str">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="M2398" t="str">
+        <f t="shared" si="118"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:13">
+      <c r="A2399" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2399" s="7">
+        <v>181</v>
+      </c>
+      <c r="C2399">
+        <v>6</v>
+      </c>
+      <c r="D2399" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2399">
+        <v>1</v>
+      </c>
+      <c r="F2399" t="s">
+        <v>572</v>
+      </c>
+      <c r="H2399" t="s">
+        <v>540</v>
+      </c>
+      <c r="I2399">
+        <v>1</v>
+      </c>
+      <c r="J2399">
+        <v>2</v>
+      </c>
+      <c r="K2399">
+        <v>0</v>
+      </c>
+      <c r="L2399" t="str">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="M2399" t="str">
+        <f t="shared" si="118"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:13">
+      <c r="A2400" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2400" s="7">
+        <v>181</v>
+      </c>
+      <c r="C2400">
+        <v>7</v>
+      </c>
+      <c r="D2400" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2400">
+        <v>1</v>
+      </c>
+      <c r="F2400" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2400" t="s">
+        <v>141</v>
+      </c>
+      <c r="I2400">
+        <v>1</v>
+      </c>
+      <c r="J2400">
+        <v>2</v>
+      </c>
+      <c r="K2400">
+        <v>0</v>
+      </c>
+      <c r="L2400" t="str">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="M2400" t="str">
+        <f t="shared" si="118"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:13">
+      <c r="A2401" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2401" s="7">
+        <v>181</v>
+      </c>
+      <c r="C2401">
+        <v>8</v>
+      </c>
+      <c r="D2401" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2401">
+        <v>1</v>
+      </c>
+      <c r="F2401" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2401" t="s">
+        <v>568</v>
+      </c>
+      <c r="I2401">
+        <v>1</v>
+      </c>
+      <c r="J2401">
+        <v>2</v>
+      </c>
+      <c r="K2401">
+        <v>0</v>
+      </c>
+      <c r="L2401" t="str">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="M2401" t="str">
+        <f t="shared" si="118"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2402" spans="1:13">
+      <c r="A2402" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2402" s="7">
+        <v>181</v>
+      </c>
+      <c r="C2402">
+        <v>9</v>
+      </c>
+      <c r="D2402" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2402">
+        <v>1</v>
+      </c>
+      <c r="F2402" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2402" t="s">
+        <v>581</v>
+      </c>
+      <c r="I2402">
+        <v>1</v>
+      </c>
+      <c r="J2402">
+        <v>2</v>
+      </c>
+      <c r="K2402">
+        <v>0</v>
+      </c>
+      <c r="L2402" t="str">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="M2402" t="str">
+        <f t="shared" si="118"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2403" spans="1:13">
+      <c r="A2403" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2403" s="7">
+        <v>181</v>
+      </c>
+      <c r="C2403">
+        <v>10</v>
+      </c>
+      <c r="D2403" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2403">
+        <v>1</v>
+      </c>
+      <c r="F2403" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2403" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2403">
+        <v>1</v>
+      </c>
+      <c r="J2403">
+        <v>2</v>
+      </c>
+      <c r="K2403">
+        <v>0</v>
+      </c>
+      <c r="L2403" t="str">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="M2403" t="str">
+        <f t="shared" si="118"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:13">
+      <c r="A2404" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2404" s="7">
+        <v>181</v>
+      </c>
+      <c r="C2404">
+        <v>11</v>
+      </c>
+      <c r="D2404" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2404">
+        <v>1</v>
+      </c>
+      <c r="F2404" t="s">
+        <v>377</v>
+      </c>
+      <c r="H2404" t="s">
+        <v>263</v>
+      </c>
+      <c r="I2404">
+        <v>1</v>
+      </c>
+      <c r="J2404">
+        <v>2</v>
+      </c>
+      <c r="K2404">
+        <v>0</v>
+      </c>
+      <c r="L2404" t="str">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="M2404" t="str">
+        <f t="shared" si="118"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:13">
+      <c r="A2405" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2405" s="7">
+        <v>181</v>
+      </c>
+      <c r="C2405">
+        <v>12</v>
+      </c>
+      <c r="D2405" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2405">
+        <v>1</v>
+      </c>
+      <c r="F2405" t="s">
+        <v>206</v>
+      </c>
+      <c r="H2405" t="s">
+        <v>483</v>
+      </c>
+      <c r="I2405">
+        <v>0</v>
+      </c>
+      <c r="J2405">
+        <v>3</v>
+      </c>
+      <c r="K2405">
+        <v>0</v>
+      </c>
+      <c r="L2405" t="str">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="M2405" t="str">
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new data 2026 02 06
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9742" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9808" uniqueCount="636">
   <si>
     <t>Fecha</t>
   </si>
@@ -1930,6 +1930,18 @@
   <si>
     <t>monster</t>
   </si>
+  <si>
+    <t>2026.02.06</t>
+  </si>
+  <si>
+    <t>Francisco Miranda</t>
+  </si>
+  <si>
+    <t>Rodrigo Ferry</t>
+  </si>
+  <si>
+    <t>Rodrigo Silva</t>
+  </si>
 </sst>
 </file>
 
@@ -2263,13 +2275,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2405"/>
+  <dimension ref="A1:M2421"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2384" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2396" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F2406" sqref="F2406"/>
+      <selection pane="bottomRight" activeCell="F2419" sqref="F2419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -98878,6 +98890,652 @@
       </c>
       <c r="M2405" t="str">
         <f t="shared" si="118"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:13">
+      <c r="A2406" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2406" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2406">
+        <v>1</v>
+      </c>
+      <c r="D2406" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2406">
+        <v>1</v>
+      </c>
+      <c r="F2406" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2406" t="s">
+        <v>631</v>
+      </c>
+      <c r="H2406" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2406">
+        <v>3</v>
+      </c>
+      <c r="J2406">
+        <v>0</v>
+      </c>
+      <c r="K2406">
+        <v>0</v>
+      </c>
+      <c r="L2406" t="str">
+        <f t="shared" ref="L2406:L2421" si="119">IF(C2406=1,"1",IF(C2406=2,"1",IF(C2406=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2406" t="str">
+        <f t="shared" ref="M2406:M2421" si="120">IF(C2406=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:13">
+      <c r="A2407" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2407" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2407">
+        <v>2</v>
+      </c>
+      <c r="D2407" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2407">
+        <v>1</v>
+      </c>
+      <c r="F2407" t="s">
+        <v>396</v>
+      </c>
+      <c r="H2407" t="s">
+        <v>568</v>
+      </c>
+      <c r="I2407">
+        <v>2</v>
+      </c>
+      <c r="J2407">
+        <v>0</v>
+      </c>
+      <c r="K2407">
+        <v>1</v>
+      </c>
+      <c r="L2407" t="str">
+        <f t="shared" si="119"/>
+        <v>1</v>
+      </c>
+      <c r="M2407" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:13">
+      <c r="A2408" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2408" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2408">
+        <v>3</v>
+      </c>
+      <c r="D2408" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2408">
+        <v>1</v>
+      </c>
+      <c r="F2408" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2408" t="s">
+        <v>633</v>
+      </c>
+      <c r="I2408">
+        <v>2</v>
+      </c>
+      <c r="J2408">
+        <v>1</v>
+      </c>
+      <c r="K2408">
+        <v>0</v>
+      </c>
+      <c r="L2408" t="str">
+        <f t="shared" si="119"/>
+        <v>1</v>
+      </c>
+      <c r="M2408" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:13">
+      <c r="A2409" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2409" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2409">
+        <v>4</v>
+      </c>
+      <c r="D2409" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2409">
+        <v>1</v>
+      </c>
+      <c r="F2409" t="s">
+        <v>572</v>
+      </c>
+      <c r="H2409" t="s">
+        <v>540</v>
+      </c>
+      <c r="I2409">
+        <v>2</v>
+      </c>
+      <c r="J2409">
+        <v>1</v>
+      </c>
+      <c r="K2409">
+        <v>0</v>
+      </c>
+      <c r="L2409" t="str">
+        <f t="shared" si="119"/>
+        <v>0</v>
+      </c>
+      <c r="M2409" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:13">
+      <c r="A2410" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2410" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2410">
+        <v>5</v>
+      </c>
+      <c r="D2410" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2410">
+        <v>1</v>
+      </c>
+      <c r="F2410" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2410" t="s">
+        <v>634</v>
+      </c>
+      <c r="I2410">
+        <v>2</v>
+      </c>
+      <c r="J2410">
+        <v>1</v>
+      </c>
+      <c r="K2410">
+        <v>0</v>
+      </c>
+      <c r="L2410" t="str">
+        <f t="shared" si="119"/>
+        <v>0</v>
+      </c>
+      <c r="M2410" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:13">
+      <c r="A2411" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2411" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2411">
+        <v>6</v>
+      </c>
+      <c r="D2411" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2411">
+        <v>1</v>
+      </c>
+      <c r="F2411" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2411" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2411">
+        <v>2</v>
+      </c>
+      <c r="J2411">
+        <v>1</v>
+      </c>
+      <c r="K2411">
+        <v>0</v>
+      </c>
+      <c r="L2411" t="str">
+        <f t="shared" si="119"/>
+        <v>0</v>
+      </c>
+      <c r="M2411" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:13">
+      <c r="A2412" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2412" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2412">
+        <v>7</v>
+      </c>
+      <c r="D2412" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2412">
+        <v>1</v>
+      </c>
+      <c r="F2412" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2412" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2412">
+        <v>2</v>
+      </c>
+      <c r="J2412">
+        <v>1</v>
+      </c>
+      <c r="K2412">
+        <v>0</v>
+      </c>
+      <c r="L2412" t="str">
+        <f t="shared" si="119"/>
+        <v>0</v>
+      </c>
+      <c r="M2412" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2413" spans="1:13">
+      <c r="A2413" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2413" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2413">
+        <v>8</v>
+      </c>
+      <c r="D2413" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2413">
+        <v>1</v>
+      </c>
+      <c r="F2413" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2413" t="s">
+        <v>631</v>
+      </c>
+      <c r="H2413" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2413">
+        <v>1</v>
+      </c>
+      <c r="J2413">
+        <v>0</v>
+      </c>
+      <c r="K2413">
+        <v>2</v>
+      </c>
+      <c r="L2413" t="str">
+        <f t="shared" si="119"/>
+        <v>0</v>
+      </c>
+      <c r="M2413" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2414" spans="1:13">
+      <c r="A2414" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2414" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2414">
+        <v>9</v>
+      </c>
+      <c r="D2414" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2414">
+        <v>1</v>
+      </c>
+      <c r="F2414" t="s">
+        <v>548</v>
+      </c>
+      <c r="H2414" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2414">
+        <v>1</v>
+      </c>
+      <c r="J2414">
+        <v>2</v>
+      </c>
+      <c r="K2414">
+        <v>0</v>
+      </c>
+      <c r="L2414" t="str">
+        <f t="shared" si="119"/>
+        <v>0</v>
+      </c>
+      <c r="M2414" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:13">
+      <c r="A2415" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2415" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2415">
+        <v>10</v>
+      </c>
+      <c r="D2415" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2415">
+        <v>1</v>
+      </c>
+      <c r="F2415" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2415" t="s">
+        <v>201</v>
+      </c>
+      <c r="I2415">
+        <v>1</v>
+      </c>
+      <c r="J2415">
+        <v>2</v>
+      </c>
+      <c r="K2415">
+        <v>0</v>
+      </c>
+      <c r="L2415" t="str">
+        <f t="shared" si="119"/>
+        <v>0</v>
+      </c>
+      <c r="M2415" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:13">
+      <c r="A2416" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2416" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2416">
+        <v>11</v>
+      </c>
+      <c r="D2416" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2416">
+        <v>1</v>
+      </c>
+      <c r="F2416" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2416" t="s">
+        <v>635</v>
+      </c>
+      <c r="I2416">
+        <v>1</v>
+      </c>
+      <c r="J2416">
+        <v>2</v>
+      </c>
+      <c r="K2416">
+        <v>0</v>
+      </c>
+      <c r="L2416" t="str">
+        <f t="shared" si="119"/>
+        <v>0</v>
+      </c>
+      <c r="M2416" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:13">
+      <c r="A2417" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2417" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2417">
+        <v>12</v>
+      </c>
+      <c r="D2417" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2417">
+        <v>1</v>
+      </c>
+      <c r="F2417" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2417" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2417">
+        <v>1</v>
+      </c>
+      <c r="J2417">
+        <v>2</v>
+      </c>
+      <c r="K2417">
+        <v>0</v>
+      </c>
+      <c r="L2417" t="str">
+        <f t="shared" si="119"/>
+        <v>0</v>
+      </c>
+      <c r="M2417" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:13">
+      <c r="A2418" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2418" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2418">
+        <v>13</v>
+      </c>
+      <c r="D2418" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2418">
+        <v>1</v>
+      </c>
+      <c r="F2418" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2418" t="s">
+        <v>301</v>
+      </c>
+      <c r="I2418">
+        <v>1</v>
+      </c>
+      <c r="J2418">
+        <v>2</v>
+      </c>
+      <c r="K2418">
+        <v>0</v>
+      </c>
+      <c r="L2418" t="str">
+        <f t="shared" si="119"/>
+        <v>0</v>
+      </c>
+      <c r="M2418" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2419" spans="1:13">
+      <c r="A2419" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2419" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2419">
+        <v>14</v>
+      </c>
+      <c r="D2419" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2419">
+        <v>1</v>
+      </c>
+      <c r="F2419" t="s">
+        <v>163</v>
+      </c>
+      <c r="H2419" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2419">
+        <v>1</v>
+      </c>
+      <c r="J2419">
+        <v>2</v>
+      </c>
+      <c r="K2419">
+        <v>0</v>
+      </c>
+      <c r="L2419" t="str">
+        <f t="shared" si="119"/>
+        <v>0</v>
+      </c>
+      <c r="M2419" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2420" spans="1:13">
+      <c r="A2420" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2420" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2420">
+        <v>15</v>
+      </c>
+      <c r="D2420" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2420">
+        <v>1</v>
+      </c>
+      <c r="F2420" t="s">
+        <v>572</v>
+      </c>
+      <c r="H2420" t="s">
+        <v>532</v>
+      </c>
+      <c r="I2420">
+        <v>0</v>
+      </c>
+      <c r="J2420">
+        <v>3</v>
+      </c>
+      <c r="K2420">
+        <v>0</v>
+      </c>
+      <c r="L2420" t="str">
+        <f t="shared" si="119"/>
+        <v>0</v>
+      </c>
+      <c r="M2420" t="str">
+        <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:13">
+      <c r="A2421" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2421" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2421">
+        <v>16</v>
+      </c>
+      <c r="D2421" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2421">
+        <v>1</v>
+      </c>
+      <c r="F2421" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2421" t="s">
+        <v>578</v>
+      </c>
+      <c r="I2421">
+        <v>0</v>
+      </c>
+      <c r="J2421">
+        <v>3</v>
+      </c>
+      <c r="K2421">
+        <v>0</v>
+      </c>
+      <c r="L2421" t="str">
+        <f t="shared" si="119"/>
+        <v>0</v>
+      </c>
+      <c r="M2421" t="str">
+        <f t="shared" si="120"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new data 2026 02 10
</commit_message>
<xml_diff>
--- a/metaR.xlsx
+++ b/metaR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9808" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9864" uniqueCount="637">
   <si>
     <t>Fecha</t>
   </si>
@@ -1942,6 +1942,9 @@
   <si>
     <t>Rodrigo Silva</t>
   </si>
+  <si>
+    <t>2026.02.10</t>
+  </si>
 </sst>
 </file>
 
@@ -2275,13 +2278,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2421"/>
+  <dimension ref="A1:M2435"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2396" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2414" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A1965" sqref="A1965"/>
-      <selection pane="bottomRight" activeCell="F2419" sqref="F2419"/>
+      <selection pane="bottomRight" activeCell="F2429" sqref="F2429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -99536,6 +99539,566 @@
       </c>
       <c r="M2421" t="str">
         <f t="shared" si="120"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:13">
+      <c r="A2422" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2422" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2422">
+        <v>1</v>
+      </c>
+      <c r="D2422" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2422">
+        <v>1</v>
+      </c>
+      <c r="F2422" t="s">
+        <v>510</v>
+      </c>
+      <c r="H2422" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2422">
+        <v>3</v>
+      </c>
+      <c r="J2422">
+        <v>0</v>
+      </c>
+      <c r="K2422">
+        <v>0</v>
+      </c>
+      <c r="L2422" t="str">
+        <f t="shared" ref="L2422:L2435" si="121">IF(C2422=1,"1",IF(C2422=2,"1",IF(C2422=3,"1","0")))</f>
+        <v>1</v>
+      </c>
+      <c r="M2422" t="str">
+        <f t="shared" ref="M2422:M2435" si="122">IF(C2422=1,"1","0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:13">
+      <c r="A2423" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2423" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2423">
+        <v>2</v>
+      </c>
+      <c r="D2423" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2423">
+        <v>1</v>
+      </c>
+      <c r="F2423" t="s">
+        <v>572</v>
+      </c>
+      <c r="H2423" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2423">
+        <v>2</v>
+      </c>
+      <c r="J2423">
+        <v>0</v>
+      </c>
+      <c r="K2423">
+        <v>1</v>
+      </c>
+      <c r="L2423" t="str">
+        <f t="shared" si="121"/>
+        <v>1</v>
+      </c>
+      <c r="M2423" t="str">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:13">
+      <c r="A2424" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2424" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2424">
+        <v>3</v>
+      </c>
+      <c r="D2424" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2424">
+        <v>1</v>
+      </c>
+      <c r="F2424" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2424" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2424">
+        <v>2</v>
+      </c>
+      <c r="J2424">
+        <v>0</v>
+      </c>
+      <c r="K2424">
+        <v>1</v>
+      </c>
+      <c r="L2424" t="str">
+        <f t="shared" si="121"/>
+        <v>1</v>
+      </c>
+      <c r="M2424" t="str">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:13">
+      <c r="A2425" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2425" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2425">
+        <v>4</v>
+      </c>
+      <c r="D2425" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2425">
+        <v>1</v>
+      </c>
+      <c r="F2425" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2425" t="s">
+        <v>581</v>
+      </c>
+      <c r="I2425">
+        <v>2</v>
+      </c>
+      <c r="J2425">
+        <v>1</v>
+      </c>
+      <c r="K2425">
+        <v>0</v>
+      </c>
+      <c r="L2425" t="str">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="M2425" t="str">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:13">
+      <c r="A2426" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2426" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2426">
+        <v>5</v>
+      </c>
+      <c r="D2426" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2426">
+        <v>1</v>
+      </c>
+      <c r="F2426" t="s">
+        <v>510</v>
+      </c>
+      <c r="H2426" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2426">
+        <v>2</v>
+      </c>
+      <c r="J2426">
+        <v>1</v>
+      </c>
+      <c r="K2426">
+        <v>0</v>
+      </c>
+      <c r="L2426" t="str">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="M2426" t="str">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:13">
+      <c r="A2427" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2427" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2427">
+        <v>6</v>
+      </c>
+      <c r="D2427" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2427">
+        <v>1</v>
+      </c>
+      <c r="F2427" t="s">
+        <v>571</v>
+      </c>
+      <c r="H2427" t="s">
+        <v>635</v>
+      </c>
+      <c r="I2427">
+        <v>2</v>
+      </c>
+      <c r="J2427">
+        <v>1</v>
+      </c>
+      <c r="K2427">
+        <v>0</v>
+      </c>
+      <c r="L2427" t="str">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="M2427" t="str">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2428" spans="1:13">
+      <c r="A2428" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2428" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2428">
+        <v>7</v>
+      </c>
+      <c r="D2428" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2428">
+        <v>1</v>
+      </c>
+      <c r="F2428" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2428" t="s">
+        <v>416</v>
+      </c>
+      <c r="I2428">
+        <v>2</v>
+      </c>
+      <c r="J2428">
+        <v>1</v>
+      </c>
+      <c r="K2428">
+        <v>0</v>
+      </c>
+      <c r="L2428" t="str">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="M2428" t="str">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2429" spans="1:13">
+      <c r="A2429" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2429" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2429">
+        <v>8</v>
+      </c>
+      <c r="D2429" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2429">
+        <v>1</v>
+      </c>
+      <c r="F2429" t="s">
+        <v>510</v>
+      </c>
+      <c r="H2429" t="s">
+        <v>263</v>
+      </c>
+      <c r="I2429">
+        <v>1</v>
+      </c>
+      <c r="J2429">
+        <v>2</v>
+      </c>
+      <c r="K2429">
+        <v>0</v>
+      </c>
+      <c r="L2429" t="str">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="M2429" t="str">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2430" spans="1:13">
+      <c r="A2430" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2430" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2430">
+        <v>9</v>
+      </c>
+      <c r="D2430" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2430">
+        <v>1</v>
+      </c>
+      <c r="F2430" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2430" t="s">
+        <v>214</v>
+      </c>
+      <c r="I2430">
+        <v>1</v>
+      </c>
+      <c r="J2430">
+        <v>2</v>
+      </c>
+      <c r="K2430">
+        <v>0</v>
+      </c>
+      <c r="L2430" t="str">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="M2430" t="str">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2431" spans="1:13">
+      <c r="A2431" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2431" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2431">
+        <v>10</v>
+      </c>
+      <c r="D2431" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2431">
+        <v>1</v>
+      </c>
+      <c r="F2431" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2431" t="s">
+        <v>568</v>
+      </c>
+      <c r="I2431">
+        <v>1</v>
+      </c>
+      <c r="J2431">
+        <v>2</v>
+      </c>
+      <c r="K2431">
+        <v>0</v>
+      </c>
+      <c r="L2431" t="str">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="M2431" t="str">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2432" spans="1:13">
+      <c r="A2432" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2432" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2432">
+        <v>11</v>
+      </c>
+      <c r="D2432" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2432">
+        <v>1</v>
+      </c>
+      <c r="F2432" t="s">
+        <v>163</v>
+      </c>
+      <c r="H2432" t="s">
+        <v>532</v>
+      </c>
+      <c r="I2432">
+        <v>1</v>
+      </c>
+      <c r="J2432">
+        <v>2</v>
+      </c>
+      <c r="K2432">
+        <v>0</v>
+      </c>
+      <c r="L2432" t="str">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="M2432" t="str">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2433" spans="1:13">
+      <c r="A2433" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2433" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2433">
+        <v>12</v>
+      </c>
+      <c r="D2433" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2433">
+        <v>1</v>
+      </c>
+      <c r="F2433" t="s">
+        <v>603</v>
+      </c>
+      <c r="H2433" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2433">
+        <v>0</v>
+      </c>
+      <c r="J2433">
+        <v>2</v>
+      </c>
+      <c r="K2433">
+        <v>1</v>
+      </c>
+      <c r="L2433" t="str">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="M2433" t="str">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:13">
+      <c r="A2434" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2434" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2434">
+        <v>13</v>
+      </c>
+      <c r="D2434" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2434">
+        <v>1</v>
+      </c>
+      <c r="F2434" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2434" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2434">
+        <v>0</v>
+      </c>
+      <c r="J2434">
+        <v>2</v>
+      </c>
+      <c r="K2434">
+        <v>1</v>
+      </c>
+      <c r="L2434" t="str">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="M2434" t="str">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:13">
+      <c r="A2435" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2435" s="7">
+        <v>183</v>
+      </c>
+      <c r="C2435">
+        <v>14</v>
+      </c>
+      <c r="D2435" t="s">
+        <v>630</v>
+      </c>
+      <c r="E2435">
+        <v>1</v>
+      </c>
+      <c r="F2435" t="s">
+        <v>206</v>
+      </c>
+      <c r="H2435" t="s">
+        <v>483</v>
+      </c>
+      <c r="I2435">
+        <v>0</v>
+      </c>
+      <c r="J2435">
+        <v>2</v>
+      </c>
+      <c r="K2435">
+        <v>0</v>
+      </c>
+      <c r="L2435" t="str">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="M2435" t="str">
+        <f t="shared" si="122"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>